<commit_message>
Updated BinaryTrees.xls  and CheckingAndPrinting
</commit_message>
<xml_diff>
--- a/resources/BinaryTrees.xlsx
+++ b/resources/BinaryTrees.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TraversalAndView" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="383">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -714,19 +714,26 @@
 checkIfRemovingAnEdgeInBinaryTreeCanDivideItIntoTwoHalvesWithEqualSizeBottomUp</t>
   </si>
   <si>
+    <t xml:space="preserve">Print cousins of a given node in Binary Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Printing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">printCousinsOfGivenNodeWithRecursion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print cousins of a given node in Binary Tree | Single Traversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">printCousinsOfGivenNodeWithoutRecursionWithQueueApproach1
+PrintCousinsOfGivenNodeWithoutRecursionWithQueueApproach2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Print Sibling Of Node In BinaryTree</t>
   </si>
   <si>
-    <t xml:space="preserve">Printing</t>
-  </si>
-  <si>
     <t xml:space="preserve">printSiblingOfNodeInBinaryTree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print cousins of a given node in Binary Tree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print cousins of a given node in Binary Tree | Single Traversal</t>
   </si>
   <si>
     <t xml:space="preserve">Print all nodes that don’t have sibling</t>
@@ -861,6 +868,9 @@
   </si>
   <si>
     <t xml:space="preserve">Print Binary Tree levels in sorted order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">printElementsInEachLevelInSortedOrderWithoutRecursionWithPriorityQueue</t>
   </si>
   <si>
     <t xml:space="preserve">Print Binary Tree levels in sorted order | Set 2 (Using set)</t>
@@ -1298,7 +1308,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1344,12 +1354,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1397,7 +1401,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1442,10 +1446,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1454,7 +1454,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3099,13 +3099,13 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:AMJ82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D46" activeCellId="0" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="9"/>
@@ -3116,7 +3116,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="10" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>165</v>
       </c>
@@ -3158,7 +3158,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>169</v>
       </c>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>171</v>
       </c>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>173</v>
       </c>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>175</v>
       </c>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>177</v>
       </c>
@@ -3253,7 +3253,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>180</v>
       </c>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>182</v>
       </c>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
         <v>184</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>186</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
         <v>188</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>190</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
         <v>193</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
         <v>195</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
         <v>197</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
         <v>200</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
         <v>202</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
         <v>205</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
         <v>207</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
         <v>208</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
         <v>209</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
         <v>210</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="55.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
         <v>212</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
         <v>214</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
         <v>217</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
         <v>219</v>
       </c>
@@ -3588,8 +3588,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+    <row r="28" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="s">
         <v>221</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -3598,14 +3598,14 @@
       <c r="C28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="10" t="s">
         <v>223</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
         <v>224</v>
       </c>
@@ -3615,13 +3615,16 @@
       <c r="C29" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="D29" s="2" t="s">
+        <v>225</v>
+      </c>
       <c r="F29" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
-        <v>225</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>222</v>
@@ -3629,13 +3632,16 @@
       <c r="C30" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="D30" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="F30" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>222</v>
@@ -3644,15 +3650,15 @@
         <v>65</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>222</v>
@@ -3661,15 +3667,15 @@
         <v>215</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>222</v>
@@ -3678,15 +3684,15 @@
         <v>215</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>222</v>
@@ -3695,15 +3701,15 @@
         <v>215</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>222</v>
@@ -3715,9 +3721,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>222</v>
@@ -3729,9 +3735,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>222</v>
@@ -3740,15 +3746,15 @@
         <v>215</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>222</v>
@@ -3760,426 +3766,438 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F40" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="7" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F42" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>252</v>
+        <v>254</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F46" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D50" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="F50" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="11" t="s">
-        <v>265</v>
+    </row>
+    <row r="51" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="7" t="s">
+        <v>267</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>272</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>258</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F58" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="7" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F62" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F63" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F64" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F65" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="7" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>222</v>
@@ -4191,7 +4209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7" t="s">
         <v>180</v>
       </c>
@@ -4205,9 +4223,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="7" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>222</v>
@@ -4218,6 +4236,1032 @@
       <c r="F68" s="10" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0"/>
+      <c r="B82" s="0"/>
+      <c r="C82" s="0"/>
+      <c r="D82" s="0"/>
+      <c r="E82" s="0"/>
+      <c r="F82" s="0"/>
+      <c r="G82" s="0"/>
+      <c r="H82" s="0"/>
+      <c r="I82" s="0"/>
+      <c r="J82" s="0"/>
+      <c r="K82" s="0"/>
+      <c r="L82" s="0"/>
+      <c r="M82" s="0"/>
+      <c r="N82" s="0"/>
+      <c r="O82" s="0"/>
+      <c r="P82" s="0"/>
+      <c r="Q82" s="0"/>
+      <c r="R82" s="0"/>
+      <c r="S82" s="0"/>
+      <c r="T82" s="0"/>
+      <c r="U82" s="0"/>
+      <c r="V82" s="0"/>
+      <c r="W82" s="0"/>
+      <c r="X82" s="0"/>
+      <c r="Y82" s="0"/>
+      <c r="Z82" s="0"/>
+      <c r="AA82" s="0"/>
+      <c r="AB82" s="0"/>
+      <c r="AC82" s="0"/>
+      <c r="AD82" s="0"/>
+      <c r="AE82" s="0"/>
+      <c r="AF82" s="0"/>
+      <c r="AG82" s="0"/>
+      <c r="AH82" s="0"/>
+      <c r="AI82" s="0"/>
+      <c r="AJ82" s="0"/>
+      <c r="AK82" s="0"/>
+      <c r="AL82" s="0"/>
+      <c r="AM82" s="0"/>
+      <c r="AN82" s="0"/>
+      <c r="AO82" s="0"/>
+      <c r="AP82" s="0"/>
+      <c r="AQ82" s="0"/>
+      <c r="AR82" s="0"/>
+      <c r="AS82" s="0"/>
+      <c r="AT82" s="0"/>
+      <c r="AU82" s="0"/>
+      <c r="AV82" s="0"/>
+      <c r="AW82" s="0"/>
+      <c r="AX82" s="0"/>
+      <c r="AY82" s="0"/>
+      <c r="AZ82" s="0"/>
+      <c r="BA82" s="0"/>
+      <c r="BB82" s="0"/>
+      <c r="BC82" s="0"/>
+      <c r="BD82" s="0"/>
+      <c r="BE82" s="0"/>
+      <c r="BF82" s="0"/>
+      <c r="BG82" s="0"/>
+      <c r="BH82" s="0"/>
+      <c r="BI82" s="0"/>
+      <c r="BJ82" s="0"/>
+      <c r="BK82" s="0"/>
+      <c r="BL82" s="0"/>
+      <c r="BM82" s="0"/>
+      <c r="BN82" s="0"/>
+      <c r="BO82" s="0"/>
+      <c r="BP82" s="0"/>
+      <c r="BQ82" s="0"/>
+      <c r="BR82" s="0"/>
+      <c r="BS82" s="0"/>
+      <c r="BT82" s="0"/>
+      <c r="BU82" s="0"/>
+      <c r="BV82" s="0"/>
+      <c r="BW82" s="0"/>
+      <c r="BX82" s="0"/>
+      <c r="BY82" s="0"/>
+      <c r="BZ82" s="0"/>
+      <c r="CA82" s="0"/>
+      <c r="CB82" s="0"/>
+      <c r="CC82" s="0"/>
+      <c r="CD82" s="0"/>
+      <c r="CE82" s="0"/>
+      <c r="CF82" s="0"/>
+      <c r="CG82" s="0"/>
+      <c r="CH82" s="0"/>
+      <c r="CI82" s="0"/>
+      <c r="CJ82" s="0"/>
+      <c r="CK82" s="0"/>
+      <c r="CL82" s="0"/>
+      <c r="CM82" s="0"/>
+      <c r="CN82" s="0"/>
+      <c r="CO82" s="0"/>
+      <c r="CP82" s="0"/>
+      <c r="CQ82" s="0"/>
+      <c r="CR82" s="0"/>
+      <c r="CS82" s="0"/>
+      <c r="CT82" s="0"/>
+      <c r="CU82" s="0"/>
+      <c r="CV82" s="0"/>
+      <c r="CW82" s="0"/>
+      <c r="CX82" s="0"/>
+      <c r="CY82" s="0"/>
+      <c r="CZ82" s="0"/>
+      <c r="DA82" s="0"/>
+      <c r="DB82" s="0"/>
+      <c r="DC82" s="0"/>
+      <c r="DD82" s="0"/>
+      <c r="DE82" s="0"/>
+      <c r="DF82" s="0"/>
+      <c r="DG82" s="0"/>
+      <c r="DH82" s="0"/>
+      <c r="DI82" s="0"/>
+      <c r="DJ82" s="0"/>
+      <c r="DK82" s="0"/>
+      <c r="DL82" s="0"/>
+      <c r="DM82" s="0"/>
+      <c r="DN82" s="0"/>
+      <c r="DO82" s="0"/>
+      <c r="DP82" s="0"/>
+      <c r="DQ82" s="0"/>
+      <c r="DR82" s="0"/>
+      <c r="DS82" s="0"/>
+      <c r="DT82" s="0"/>
+      <c r="DU82" s="0"/>
+      <c r="DV82" s="0"/>
+      <c r="DW82" s="0"/>
+      <c r="DX82" s="0"/>
+      <c r="DY82" s="0"/>
+      <c r="DZ82" s="0"/>
+      <c r="EA82" s="0"/>
+      <c r="EB82" s="0"/>
+      <c r="EC82" s="0"/>
+      <c r="ED82" s="0"/>
+      <c r="EE82" s="0"/>
+      <c r="EF82" s="0"/>
+      <c r="EG82" s="0"/>
+      <c r="EH82" s="0"/>
+      <c r="EI82" s="0"/>
+      <c r="EJ82" s="0"/>
+      <c r="EK82" s="0"/>
+      <c r="EL82" s="0"/>
+      <c r="EM82" s="0"/>
+      <c r="EN82" s="0"/>
+      <c r="EO82" s="0"/>
+      <c r="EP82" s="0"/>
+      <c r="EQ82" s="0"/>
+      <c r="ER82" s="0"/>
+      <c r="ES82" s="0"/>
+      <c r="ET82" s="0"/>
+      <c r="EU82" s="0"/>
+      <c r="EV82" s="0"/>
+      <c r="EW82" s="0"/>
+      <c r="EX82" s="0"/>
+      <c r="EY82" s="0"/>
+      <c r="EZ82" s="0"/>
+      <c r="FA82" s="0"/>
+      <c r="FB82" s="0"/>
+      <c r="FC82" s="0"/>
+      <c r="FD82" s="0"/>
+      <c r="FE82" s="0"/>
+      <c r="FF82" s="0"/>
+      <c r="FG82" s="0"/>
+      <c r="FH82" s="0"/>
+      <c r="FI82" s="0"/>
+      <c r="FJ82" s="0"/>
+      <c r="FK82" s="0"/>
+      <c r="FL82" s="0"/>
+      <c r="FM82" s="0"/>
+      <c r="FN82" s="0"/>
+      <c r="FO82" s="0"/>
+      <c r="FP82" s="0"/>
+      <c r="FQ82" s="0"/>
+      <c r="FR82" s="0"/>
+      <c r="FS82" s="0"/>
+      <c r="FT82" s="0"/>
+      <c r="FU82" s="0"/>
+      <c r="FV82" s="0"/>
+      <c r="FW82" s="0"/>
+      <c r="FX82" s="0"/>
+      <c r="FY82" s="0"/>
+      <c r="FZ82" s="0"/>
+      <c r="GA82" s="0"/>
+      <c r="GB82" s="0"/>
+      <c r="GC82" s="0"/>
+      <c r="GD82" s="0"/>
+      <c r="GE82" s="0"/>
+      <c r="GF82" s="0"/>
+      <c r="GG82" s="0"/>
+      <c r="GH82" s="0"/>
+      <c r="GI82" s="0"/>
+      <c r="GJ82" s="0"/>
+      <c r="GK82" s="0"/>
+      <c r="GL82" s="0"/>
+      <c r="GM82" s="0"/>
+      <c r="GN82" s="0"/>
+      <c r="GO82" s="0"/>
+      <c r="GP82" s="0"/>
+      <c r="GQ82" s="0"/>
+      <c r="GR82" s="0"/>
+      <c r="GS82" s="0"/>
+      <c r="GT82" s="0"/>
+      <c r="GU82" s="0"/>
+      <c r="GV82" s="0"/>
+      <c r="GW82" s="0"/>
+      <c r="GX82" s="0"/>
+      <c r="GY82" s="0"/>
+      <c r="GZ82" s="0"/>
+      <c r="HA82" s="0"/>
+      <c r="HB82" s="0"/>
+      <c r="HC82" s="0"/>
+      <c r="HD82" s="0"/>
+      <c r="HE82" s="0"/>
+      <c r="HF82" s="0"/>
+      <c r="HG82" s="0"/>
+      <c r="HH82" s="0"/>
+      <c r="HI82" s="0"/>
+      <c r="HJ82" s="0"/>
+      <c r="HK82" s="0"/>
+      <c r="HL82" s="0"/>
+      <c r="HM82" s="0"/>
+      <c r="HN82" s="0"/>
+      <c r="HO82" s="0"/>
+      <c r="HP82" s="0"/>
+      <c r="HQ82" s="0"/>
+      <c r="HR82" s="0"/>
+      <c r="HS82" s="0"/>
+      <c r="HT82" s="0"/>
+      <c r="HU82" s="0"/>
+      <c r="HV82" s="0"/>
+      <c r="HW82" s="0"/>
+      <c r="HX82" s="0"/>
+      <c r="HY82" s="0"/>
+      <c r="HZ82" s="0"/>
+      <c r="IA82" s="0"/>
+      <c r="IB82" s="0"/>
+      <c r="IC82" s="0"/>
+      <c r="ID82" s="0"/>
+      <c r="IE82" s="0"/>
+      <c r="IF82" s="0"/>
+      <c r="IG82" s="0"/>
+      <c r="IH82" s="0"/>
+      <c r="II82" s="0"/>
+      <c r="IJ82" s="0"/>
+      <c r="IK82" s="0"/>
+      <c r="IL82" s="0"/>
+      <c r="IM82" s="0"/>
+      <c r="IN82" s="0"/>
+      <c r="IO82" s="0"/>
+      <c r="IP82" s="0"/>
+      <c r="IQ82" s="0"/>
+      <c r="IR82" s="0"/>
+      <c r="IS82" s="0"/>
+      <c r="IT82" s="0"/>
+      <c r="IU82" s="0"/>
+      <c r="IV82" s="0"/>
+      <c r="IW82" s="0"/>
+      <c r="IX82" s="0"/>
+      <c r="IY82" s="0"/>
+      <c r="IZ82" s="0"/>
+      <c r="JA82" s="0"/>
+      <c r="JB82" s="0"/>
+      <c r="JC82" s="0"/>
+      <c r="JD82" s="0"/>
+      <c r="JE82" s="0"/>
+      <c r="JF82" s="0"/>
+      <c r="JG82" s="0"/>
+      <c r="JH82" s="0"/>
+      <c r="JI82" s="0"/>
+      <c r="JJ82" s="0"/>
+      <c r="JK82" s="0"/>
+      <c r="JL82" s="0"/>
+      <c r="JM82" s="0"/>
+      <c r="JN82" s="0"/>
+      <c r="JO82" s="0"/>
+      <c r="JP82" s="0"/>
+      <c r="JQ82" s="0"/>
+      <c r="JR82" s="0"/>
+      <c r="JS82" s="0"/>
+      <c r="JT82" s="0"/>
+      <c r="JU82" s="0"/>
+      <c r="JV82" s="0"/>
+      <c r="JW82" s="0"/>
+      <c r="JX82" s="0"/>
+      <c r="JY82" s="0"/>
+      <c r="JZ82" s="0"/>
+      <c r="KA82" s="0"/>
+      <c r="KB82" s="0"/>
+      <c r="KC82" s="0"/>
+      <c r="KD82" s="0"/>
+      <c r="KE82" s="0"/>
+      <c r="KF82" s="0"/>
+      <c r="KG82" s="0"/>
+      <c r="KH82" s="0"/>
+      <c r="KI82" s="0"/>
+      <c r="KJ82" s="0"/>
+      <c r="KK82" s="0"/>
+      <c r="KL82" s="0"/>
+      <c r="KM82" s="0"/>
+      <c r="KN82" s="0"/>
+      <c r="KO82" s="0"/>
+      <c r="KP82" s="0"/>
+      <c r="KQ82" s="0"/>
+      <c r="KR82" s="0"/>
+      <c r="KS82" s="0"/>
+      <c r="KT82" s="0"/>
+      <c r="KU82" s="0"/>
+      <c r="KV82" s="0"/>
+      <c r="KW82" s="0"/>
+      <c r="KX82" s="0"/>
+      <c r="KY82" s="0"/>
+      <c r="KZ82" s="0"/>
+      <c r="LA82" s="0"/>
+      <c r="LB82" s="0"/>
+      <c r="LC82" s="0"/>
+      <c r="LD82" s="0"/>
+      <c r="LE82" s="0"/>
+      <c r="LF82" s="0"/>
+      <c r="LG82" s="0"/>
+      <c r="LH82" s="0"/>
+      <c r="LI82" s="0"/>
+      <c r="LJ82" s="0"/>
+      <c r="LK82" s="0"/>
+      <c r="LL82" s="0"/>
+      <c r="LM82" s="0"/>
+      <c r="LN82" s="0"/>
+      <c r="LO82" s="0"/>
+      <c r="LP82" s="0"/>
+      <c r="LQ82" s="0"/>
+      <c r="LR82" s="0"/>
+      <c r="LS82" s="0"/>
+      <c r="LT82" s="0"/>
+      <c r="LU82" s="0"/>
+      <c r="LV82" s="0"/>
+      <c r="LW82" s="0"/>
+      <c r="LX82" s="0"/>
+      <c r="LY82" s="0"/>
+      <c r="LZ82" s="0"/>
+      <c r="MA82" s="0"/>
+      <c r="MB82" s="0"/>
+      <c r="MC82" s="0"/>
+      <c r="MD82" s="0"/>
+      <c r="ME82" s="0"/>
+      <c r="MF82" s="0"/>
+      <c r="MG82" s="0"/>
+      <c r="MH82" s="0"/>
+      <c r="MI82" s="0"/>
+      <c r="MJ82" s="0"/>
+      <c r="MK82" s="0"/>
+      <c r="ML82" s="0"/>
+      <c r="MM82" s="0"/>
+      <c r="MN82" s="0"/>
+      <c r="MO82" s="0"/>
+      <c r="MP82" s="0"/>
+      <c r="MQ82" s="0"/>
+      <c r="MR82" s="0"/>
+      <c r="MS82" s="0"/>
+      <c r="MT82" s="0"/>
+      <c r="MU82" s="0"/>
+      <c r="MV82" s="0"/>
+      <c r="MW82" s="0"/>
+      <c r="MX82" s="0"/>
+      <c r="MY82" s="0"/>
+      <c r="MZ82" s="0"/>
+      <c r="NA82" s="0"/>
+      <c r="NB82" s="0"/>
+      <c r="NC82" s="0"/>
+      <c r="ND82" s="0"/>
+      <c r="NE82" s="0"/>
+      <c r="NF82" s="0"/>
+      <c r="NG82" s="0"/>
+      <c r="NH82" s="0"/>
+      <c r="NI82" s="0"/>
+      <c r="NJ82" s="0"/>
+      <c r="NK82" s="0"/>
+      <c r="NL82" s="0"/>
+      <c r="NM82" s="0"/>
+      <c r="NN82" s="0"/>
+      <c r="NO82" s="0"/>
+      <c r="NP82" s="0"/>
+      <c r="NQ82" s="0"/>
+      <c r="NR82" s="0"/>
+      <c r="NS82" s="0"/>
+      <c r="NT82" s="0"/>
+      <c r="NU82" s="0"/>
+      <c r="NV82" s="0"/>
+      <c r="NW82" s="0"/>
+      <c r="NX82" s="0"/>
+      <c r="NY82" s="0"/>
+      <c r="NZ82" s="0"/>
+      <c r="OA82" s="0"/>
+      <c r="OB82" s="0"/>
+      <c r="OC82" s="0"/>
+      <c r="OD82" s="0"/>
+      <c r="OE82" s="0"/>
+      <c r="OF82" s="0"/>
+      <c r="OG82" s="0"/>
+      <c r="OH82" s="0"/>
+      <c r="OI82" s="0"/>
+      <c r="OJ82" s="0"/>
+      <c r="OK82" s="0"/>
+      <c r="OL82" s="0"/>
+      <c r="OM82" s="0"/>
+      <c r="ON82" s="0"/>
+      <c r="OO82" s="0"/>
+      <c r="OP82" s="0"/>
+      <c r="OQ82" s="0"/>
+      <c r="OR82" s="0"/>
+      <c r="OS82" s="0"/>
+      <c r="OT82" s="0"/>
+      <c r="OU82" s="0"/>
+      <c r="OV82" s="0"/>
+      <c r="OW82" s="0"/>
+      <c r="OX82" s="0"/>
+      <c r="OY82" s="0"/>
+      <c r="OZ82" s="0"/>
+      <c r="PA82" s="0"/>
+      <c r="PB82" s="0"/>
+      <c r="PC82" s="0"/>
+      <c r="PD82" s="0"/>
+      <c r="PE82" s="0"/>
+      <c r="PF82" s="0"/>
+      <c r="PG82" s="0"/>
+      <c r="PH82" s="0"/>
+      <c r="PI82" s="0"/>
+      <c r="PJ82" s="0"/>
+      <c r="PK82" s="0"/>
+      <c r="PL82" s="0"/>
+      <c r="PM82" s="0"/>
+      <c r="PN82" s="0"/>
+      <c r="PO82" s="0"/>
+      <c r="PP82" s="0"/>
+      <c r="PQ82" s="0"/>
+      <c r="PR82" s="0"/>
+      <c r="PS82" s="0"/>
+      <c r="PT82" s="0"/>
+      <c r="PU82" s="0"/>
+      <c r="PV82" s="0"/>
+      <c r="PW82" s="0"/>
+      <c r="PX82" s="0"/>
+      <c r="PY82" s="0"/>
+      <c r="PZ82" s="0"/>
+      <c r="QA82" s="0"/>
+      <c r="QB82" s="0"/>
+      <c r="QC82" s="0"/>
+      <c r="QD82" s="0"/>
+      <c r="QE82" s="0"/>
+      <c r="QF82" s="0"/>
+      <c r="QG82" s="0"/>
+      <c r="QH82" s="0"/>
+      <c r="QI82" s="0"/>
+      <c r="QJ82" s="0"/>
+      <c r="QK82" s="0"/>
+      <c r="QL82" s="0"/>
+      <c r="QM82" s="0"/>
+      <c r="QN82" s="0"/>
+      <c r="QO82" s="0"/>
+      <c r="QP82" s="0"/>
+      <c r="QQ82" s="0"/>
+      <c r="QR82" s="0"/>
+      <c r="QS82" s="0"/>
+      <c r="QT82" s="0"/>
+      <c r="QU82" s="0"/>
+      <c r="QV82" s="0"/>
+      <c r="QW82" s="0"/>
+      <c r="QX82" s="0"/>
+      <c r="QY82" s="0"/>
+      <c r="QZ82" s="0"/>
+      <c r="RA82" s="0"/>
+      <c r="RB82" s="0"/>
+      <c r="RC82" s="0"/>
+      <c r="RD82" s="0"/>
+      <c r="RE82" s="0"/>
+      <c r="RF82" s="0"/>
+      <c r="RG82" s="0"/>
+      <c r="RH82" s="0"/>
+      <c r="RI82" s="0"/>
+      <c r="RJ82" s="0"/>
+      <c r="RK82" s="0"/>
+      <c r="RL82" s="0"/>
+      <c r="RM82" s="0"/>
+      <c r="RN82" s="0"/>
+      <c r="RO82" s="0"/>
+      <c r="RP82" s="0"/>
+      <c r="RQ82" s="0"/>
+      <c r="RR82" s="0"/>
+      <c r="RS82" s="0"/>
+      <c r="RT82" s="0"/>
+      <c r="RU82" s="0"/>
+      <c r="RV82" s="0"/>
+      <c r="RW82" s="0"/>
+      <c r="RX82" s="0"/>
+      <c r="RY82" s="0"/>
+      <c r="RZ82" s="0"/>
+      <c r="SA82" s="0"/>
+      <c r="SB82" s="0"/>
+      <c r="SC82" s="0"/>
+      <c r="SD82" s="0"/>
+      <c r="SE82" s="0"/>
+      <c r="SF82" s="0"/>
+      <c r="SG82" s="0"/>
+      <c r="SH82" s="0"/>
+      <c r="SI82" s="0"/>
+      <c r="SJ82" s="0"/>
+      <c r="SK82" s="0"/>
+      <c r="SL82" s="0"/>
+      <c r="SM82" s="0"/>
+      <c r="SN82" s="0"/>
+      <c r="SO82" s="0"/>
+      <c r="SP82" s="0"/>
+      <c r="SQ82" s="0"/>
+      <c r="SR82" s="0"/>
+      <c r="SS82" s="0"/>
+      <c r="ST82" s="0"/>
+      <c r="SU82" s="0"/>
+      <c r="SV82" s="0"/>
+      <c r="SW82" s="0"/>
+      <c r="SX82" s="0"/>
+      <c r="SY82" s="0"/>
+      <c r="SZ82" s="0"/>
+      <c r="TA82" s="0"/>
+      <c r="TB82" s="0"/>
+      <c r="TC82" s="0"/>
+      <c r="TD82" s="0"/>
+      <c r="TE82" s="0"/>
+      <c r="TF82" s="0"/>
+      <c r="TG82" s="0"/>
+      <c r="TH82" s="0"/>
+      <c r="TI82" s="0"/>
+      <c r="TJ82" s="0"/>
+      <c r="TK82" s="0"/>
+      <c r="TL82" s="0"/>
+      <c r="TM82" s="0"/>
+      <c r="TN82" s="0"/>
+      <c r="TO82" s="0"/>
+      <c r="TP82" s="0"/>
+      <c r="TQ82" s="0"/>
+      <c r="TR82" s="0"/>
+      <c r="TS82" s="0"/>
+      <c r="TT82" s="0"/>
+      <c r="TU82" s="0"/>
+      <c r="TV82" s="0"/>
+      <c r="TW82" s="0"/>
+      <c r="TX82" s="0"/>
+      <c r="TY82" s="0"/>
+      <c r="TZ82" s="0"/>
+      <c r="UA82" s="0"/>
+      <c r="UB82" s="0"/>
+      <c r="UC82" s="0"/>
+      <c r="UD82" s="0"/>
+      <c r="UE82" s="0"/>
+      <c r="UF82" s="0"/>
+      <c r="UG82" s="0"/>
+      <c r="UH82" s="0"/>
+      <c r="UI82" s="0"/>
+      <c r="UJ82" s="0"/>
+      <c r="UK82" s="0"/>
+      <c r="UL82" s="0"/>
+      <c r="UM82" s="0"/>
+      <c r="UN82" s="0"/>
+      <c r="UO82" s="0"/>
+      <c r="UP82" s="0"/>
+      <c r="UQ82" s="0"/>
+      <c r="UR82" s="0"/>
+      <c r="US82" s="0"/>
+      <c r="UT82" s="0"/>
+      <c r="UU82" s="0"/>
+      <c r="UV82" s="0"/>
+      <c r="UW82" s="0"/>
+      <c r="UX82" s="0"/>
+      <c r="UY82" s="0"/>
+      <c r="UZ82" s="0"/>
+      <c r="VA82" s="0"/>
+      <c r="VB82" s="0"/>
+      <c r="VC82" s="0"/>
+      <c r="VD82" s="0"/>
+      <c r="VE82" s="0"/>
+      <c r="VF82" s="0"/>
+      <c r="VG82" s="0"/>
+      <c r="VH82" s="0"/>
+      <c r="VI82" s="0"/>
+      <c r="VJ82" s="0"/>
+      <c r="VK82" s="0"/>
+      <c r="VL82" s="0"/>
+      <c r="VM82" s="0"/>
+      <c r="VN82" s="0"/>
+      <c r="VO82" s="0"/>
+      <c r="VP82" s="0"/>
+      <c r="VQ82" s="0"/>
+      <c r="VR82" s="0"/>
+      <c r="VS82" s="0"/>
+      <c r="VT82" s="0"/>
+      <c r="VU82" s="0"/>
+      <c r="VV82" s="0"/>
+      <c r="VW82" s="0"/>
+      <c r="VX82" s="0"/>
+      <c r="VY82" s="0"/>
+      <c r="VZ82" s="0"/>
+      <c r="WA82" s="0"/>
+      <c r="WB82" s="0"/>
+      <c r="WC82" s="0"/>
+      <c r="WD82" s="0"/>
+      <c r="WE82" s="0"/>
+      <c r="WF82" s="0"/>
+      <c r="WG82" s="0"/>
+      <c r="WH82" s="0"/>
+      <c r="WI82" s="0"/>
+      <c r="WJ82" s="0"/>
+      <c r="WK82" s="0"/>
+      <c r="WL82" s="0"/>
+      <c r="WM82" s="0"/>
+      <c r="WN82" s="0"/>
+      <c r="WO82" s="0"/>
+      <c r="WP82" s="0"/>
+      <c r="WQ82" s="0"/>
+      <c r="WR82" s="0"/>
+      <c r="WS82" s="0"/>
+      <c r="WT82" s="0"/>
+      <c r="WU82" s="0"/>
+      <c r="WV82" s="0"/>
+      <c r="WW82" s="0"/>
+      <c r="WX82" s="0"/>
+      <c r="WY82" s="0"/>
+      <c r="WZ82" s="0"/>
+      <c r="XA82" s="0"/>
+      <c r="XB82" s="0"/>
+      <c r="XC82" s="0"/>
+      <c r="XD82" s="0"/>
+      <c r="XE82" s="0"/>
+      <c r="XF82" s="0"/>
+      <c r="XG82" s="0"/>
+      <c r="XH82" s="0"/>
+      <c r="XI82" s="0"/>
+      <c r="XJ82" s="0"/>
+      <c r="XK82" s="0"/>
+      <c r="XL82" s="0"/>
+      <c r="XM82" s="0"/>
+      <c r="XN82" s="0"/>
+      <c r="XO82" s="0"/>
+      <c r="XP82" s="0"/>
+      <c r="XQ82" s="0"/>
+      <c r="XR82" s="0"/>
+      <c r="XS82" s="0"/>
+      <c r="XT82" s="0"/>
+      <c r="XU82" s="0"/>
+      <c r="XV82" s="0"/>
+      <c r="XW82" s="0"/>
+      <c r="XX82" s="0"/>
+      <c r="XY82" s="0"/>
+      <c r="XZ82" s="0"/>
+      <c r="YA82" s="0"/>
+      <c r="YB82" s="0"/>
+      <c r="YC82" s="0"/>
+      <c r="YD82" s="0"/>
+      <c r="YE82" s="0"/>
+      <c r="YF82" s="0"/>
+      <c r="YG82" s="0"/>
+      <c r="YH82" s="0"/>
+      <c r="YI82" s="0"/>
+      <c r="YJ82" s="0"/>
+      <c r="YK82" s="0"/>
+      <c r="YL82" s="0"/>
+      <c r="YM82" s="0"/>
+      <c r="YN82" s="0"/>
+      <c r="YO82" s="0"/>
+      <c r="YP82" s="0"/>
+      <c r="YQ82" s="0"/>
+      <c r="YR82" s="0"/>
+      <c r="YS82" s="0"/>
+      <c r="YT82" s="0"/>
+      <c r="YU82" s="0"/>
+      <c r="YV82" s="0"/>
+      <c r="YW82" s="0"/>
+      <c r="YX82" s="0"/>
+      <c r="YY82" s="0"/>
+      <c r="YZ82" s="0"/>
+      <c r="ZA82" s="0"/>
+      <c r="ZB82" s="0"/>
+      <c r="ZC82" s="0"/>
+      <c r="ZD82" s="0"/>
+      <c r="ZE82" s="0"/>
+      <c r="ZF82" s="0"/>
+      <c r="ZG82" s="0"/>
+      <c r="ZH82" s="0"/>
+      <c r="ZI82" s="0"/>
+      <c r="ZJ82" s="0"/>
+      <c r="ZK82" s="0"/>
+      <c r="ZL82" s="0"/>
+      <c r="ZM82" s="0"/>
+      <c r="ZN82" s="0"/>
+      <c r="ZO82" s="0"/>
+      <c r="ZP82" s="0"/>
+      <c r="ZQ82" s="0"/>
+      <c r="ZR82" s="0"/>
+      <c r="ZS82" s="0"/>
+      <c r="ZT82" s="0"/>
+      <c r="ZU82" s="0"/>
+      <c r="ZV82" s="0"/>
+      <c r="ZW82" s="0"/>
+      <c r="ZX82" s="0"/>
+      <c r="ZY82" s="0"/>
+      <c r="ZZ82" s="0"/>
+      <c r="AAA82" s="0"/>
+      <c r="AAB82" s="0"/>
+      <c r="AAC82" s="0"/>
+      <c r="AAD82" s="0"/>
+      <c r="AAE82" s="0"/>
+      <c r="AAF82" s="0"/>
+      <c r="AAG82" s="0"/>
+      <c r="AAH82" s="0"/>
+      <c r="AAI82" s="0"/>
+      <c r="AAJ82" s="0"/>
+      <c r="AAK82" s="0"/>
+      <c r="AAL82" s="0"/>
+      <c r="AAM82" s="0"/>
+      <c r="AAN82" s="0"/>
+      <c r="AAO82" s="0"/>
+      <c r="AAP82" s="0"/>
+      <c r="AAQ82" s="0"/>
+      <c r="AAR82" s="0"/>
+      <c r="AAS82" s="0"/>
+      <c r="AAT82" s="0"/>
+      <c r="AAU82" s="0"/>
+      <c r="AAV82" s="0"/>
+      <c r="AAW82" s="0"/>
+      <c r="AAX82" s="0"/>
+      <c r="AAY82" s="0"/>
+      <c r="AAZ82" s="0"/>
+      <c r="ABA82" s="0"/>
+      <c r="ABB82" s="0"/>
+      <c r="ABC82" s="0"/>
+      <c r="ABD82" s="0"/>
+      <c r="ABE82" s="0"/>
+      <c r="ABF82" s="0"/>
+      <c r="ABG82" s="0"/>
+      <c r="ABH82" s="0"/>
+      <c r="ABI82" s="0"/>
+      <c r="ABJ82" s="0"/>
+      <c r="ABK82" s="0"/>
+      <c r="ABL82" s="0"/>
+      <c r="ABM82" s="0"/>
+      <c r="ABN82" s="0"/>
+      <c r="ABO82" s="0"/>
+      <c r="ABP82" s="0"/>
+      <c r="ABQ82" s="0"/>
+      <c r="ABR82" s="0"/>
+      <c r="ABS82" s="0"/>
+      <c r="ABT82" s="0"/>
+      <c r="ABU82" s="0"/>
+      <c r="ABV82" s="0"/>
+      <c r="ABW82" s="0"/>
+      <c r="ABX82" s="0"/>
+      <c r="ABY82" s="0"/>
+      <c r="ABZ82" s="0"/>
+      <c r="ACA82" s="0"/>
+      <c r="ACB82" s="0"/>
+      <c r="ACC82" s="0"/>
+      <c r="ACD82" s="0"/>
+      <c r="ACE82" s="0"/>
+      <c r="ACF82" s="0"/>
+      <c r="ACG82" s="0"/>
+      <c r="ACH82" s="0"/>
+      <c r="ACI82" s="0"/>
+      <c r="ACJ82" s="0"/>
+      <c r="ACK82" s="0"/>
+      <c r="ACL82" s="0"/>
+      <c r="ACM82" s="0"/>
+      <c r="ACN82" s="0"/>
+      <c r="ACO82" s="0"/>
+      <c r="ACP82" s="0"/>
+      <c r="ACQ82" s="0"/>
+      <c r="ACR82" s="0"/>
+      <c r="ACS82" s="0"/>
+      <c r="ACT82" s="0"/>
+      <c r="ACU82" s="0"/>
+      <c r="ACV82" s="0"/>
+      <c r="ACW82" s="0"/>
+      <c r="ACX82" s="0"/>
+      <c r="ACY82" s="0"/>
+      <c r="ACZ82" s="0"/>
+      <c r="ADA82" s="0"/>
+      <c r="ADB82" s="0"/>
+      <c r="ADC82" s="0"/>
+      <c r="ADD82" s="0"/>
+      <c r="ADE82" s="0"/>
+      <c r="ADF82" s="0"/>
+      <c r="ADG82" s="0"/>
+      <c r="ADH82" s="0"/>
+      <c r="ADI82" s="0"/>
+      <c r="ADJ82" s="0"/>
+      <c r="ADK82" s="0"/>
+      <c r="ADL82" s="0"/>
+      <c r="ADM82" s="0"/>
+      <c r="ADN82" s="0"/>
+      <c r="ADO82" s="0"/>
+      <c r="ADP82" s="0"/>
+      <c r="ADQ82" s="0"/>
+      <c r="ADR82" s="0"/>
+      <c r="ADS82" s="0"/>
+      <c r="ADT82" s="0"/>
+      <c r="ADU82" s="0"/>
+      <c r="ADV82" s="0"/>
+      <c r="ADW82" s="0"/>
+      <c r="ADX82" s="0"/>
+      <c r="ADY82" s="0"/>
+      <c r="ADZ82" s="0"/>
+      <c r="AEA82" s="0"/>
+      <c r="AEB82" s="0"/>
+      <c r="AEC82" s="0"/>
+      <c r="AED82" s="0"/>
+      <c r="AEE82" s="0"/>
+      <c r="AEF82" s="0"/>
+      <c r="AEG82" s="0"/>
+      <c r="AEH82" s="0"/>
+      <c r="AEI82" s="0"/>
+      <c r="AEJ82" s="0"/>
+      <c r="AEK82" s="0"/>
+      <c r="AEL82" s="0"/>
+      <c r="AEM82" s="0"/>
+      <c r="AEN82" s="0"/>
+      <c r="AEO82" s="0"/>
+      <c r="AEP82" s="0"/>
+      <c r="AEQ82" s="0"/>
+      <c r="AER82" s="0"/>
+      <c r="AES82" s="0"/>
+      <c r="AET82" s="0"/>
+      <c r="AEU82" s="0"/>
+      <c r="AEV82" s="0"/>
+      <c r="AEW82" s="0"/>
+      <c r="AEX82" s="0"/>
+      <c r="AEY82" s="0"/>
+      <c r="AEZ82" s="0"/>
+      <c r="AFA82" s="0"/>
+      <c r="AFB82" s="0"/>
+      <c r="AFC82" s="0"/>
+      <c r="AFD82" s="0"/>
+      <c r="AFE82" s="0"/>
+      <c r="AFF82" s="0"/>
+      <c r="AFG82" s="0"/>
+      <c r="AFH82" s="0"/>
+      <c r="AFI82" s="0"/>
+      <c r="AFJ82" s="0"/>
+      <c r="AFK82" s="0"/>
+      <c r="AFL82" s="0"/>
+      <c r="AFM82" s="0"/>
+      <c r="AFN82" s="0"/>
+      <c r="AFO82" s="0"/>
+      <c r="AFP82" s="0"/>
+      <c r="AFQ82" s="0"/>
+      <c r="AFR82" s="0"/>
+      <c r="AFS82" s="0"/>
+      <c r="AFT82" s="0"/>
+      <c r="AFU82" s="0"/>
+      <c r="AFV82" s="0"/>
+      <c r="AFW82" s="0"/>
+      <c r="AFX82" s="0"/>
+      <c r="AFY82" s="0"/>
+      <c r="AFZ82" s="0"/>
+      <c r="AGA82" s="0"/>
+      <c r="AGB82" s="0"/>
+      <c r="AGC82" s="0"/>
+      <c r="AGD82" s="0"/>
+      <c r="AGE82" s="0"/>
+      <c r="AGF82" s="0"/>
+      <c r="AGG82" s="0"/>
+      <c r="AGH82" s="0"/>
+      <c r="AGI82" s="0"/>
+      <c r="AGJ82" s="0"/>
+      <c r="AGK82" s="0"/>
+      <c r="AGL82" s="0"/>
+      <c r="AGM82" s="0"/>
+      <c r="AGN82" s="0"/>
+      <c r="AGO82" s="0"/>
+      <c r="AGP82" s="0"/>
+      <c r="AGQ82" s="0"/>
+      <c r="AGR82" s="0"/>
+      <c r="AGS82" s="0"/>
+      <c r="AGT82" s="0"/>
+      <c r="AGU82" s="0"/>
+      <c r="AGV82" s="0"/>
+      <c r="AGW82" s="0"/>
+      <c r="AGX82" s="0"/>
+      <c r="AGY82" s="0"/>
+      <c r="AGZ82" s="0"/>
+      <c r="AHA82" s="0"/>
+      <c r="AHB82" s="0"/>
+      <c r="AHC82" s="0"/>
+      <c r="AHD82" s="0"/>
+      <c r="AHE82" s="0"/>
+      <c r="AHF82" s="0"/>
+      <c r="AHG82" s="0"/>
+      <c r="AHH82" s="0"/>
+      <c r="AHI82" s="0"/>
+      <c r="AHJ82" s="0"/>
+      <c r="AHK82" s="0"/>
+      <c r="AHL82" s="0"/>
+      <c r="AHM82" s="0"/>
+      <c r="AHN82" s="0"/>
+      <c r="AHO82" s="0"/>
+      <c r="AHP82" s="0"/>
+      <c r="AHQ82" s="0"/>
+      <c r="AHR82" s="0"/>
+      <c r="AHS82" s="0"/>
+      <c r="AHT82" s="0"/>
+      <c r="AHU82" s="0"/>
+      <c r="AHV82" s="0"/>
+      <c r="AHW82" s="0"/>
+      <c r="AHX82" s="0"/>
+      <c r="AHY82" s="0"/>
+      <c r="AHZ82" s="0"/>
+      <c r="AIA82" s="0"/>
+      <c r="AIB82" s="0"/>
+      <c r="AIC82" s="0"/>
+      <c r="AID82" s="0"/>
+      <c r="AIE82" s="0"/>
+      <c r="AIF82" s="0"/>
+      <c r="AIG82" s="0"/>
+      <c r="AIH82" s="0"/>
+      <c r="AII82" s="0"/>
+      <c r="AIJ82" s="0"/>
+      <c r="AIK82" s="0"/>
+      <c r="AIL82" s="0"/>
+      <c r="AIM82" s="0"/>
+      <c r="AIN82" s="0"/>
+      <c r="AIO82" s="0"/>
+      <c r="AIP82" s="0"/>
+      <c r="AIQ82" s="0"/>
+      <c r="AIR82" s="0"/>
+      <c r="AIS82" s="0"/>
+      <c r="AIT82" s="0"/>
+      <c r="AIU82" s="0"/>
+      <c r="AIV82" s="0"/>
+      <c r="AIW82" s="0"/>
+      <c r="AIX82" s="0"/>
+      <c r="AIY82" s="0"/>
+      <c r="AIZ82" s="0"/>
+      <c r="AJA82" s="0"/>
+      <c r="AJB82" s="0"/>
+      <c r="AJC82" s="0"/>
+      <c r="AJD82" s="0"/>
+      <c r="AJE82" s="0"/>
+      <c r="AJF82" s="0"/>
+      <c r="AJG82" s="0"/>
+      <c r="AJH82" s="0"/>
+      <c r="AJI82" s="0"/>
+      <c r="AJJ82" s="0"/>
+      <c r="AJK82" s="0"/>
+      <c r="AJL82" s="0"/>
+      <c r="AJM82" s="0"/>
+      <c r="AJN82" s="0"/>
+      <c r="AJO82" s="0"/>
+      <c r="AJP82" s="0"/>
+      <c r="AJQ82" s="0"/>
+      <c r="AJR82" s="0"/>
+      <c r="AJS82" s="0"/>
+      <c r="AJT82" s="0"/>
+      <c r="AJU82" s="0"/>
+      <c r="AJV82" s="0"/>
+      <c r="AJW82" s="0"/>
+      <c r="AJX82" s="0"/>
+      <c r="AJY82" s="0"/>
+      <c r="AJZ82" s="0"/>
+      <c r="AKA82" s="0"/>
+      <c r="AKB82" s="0"/>
+      <c r="AKC82" s="0"/>
+      <c r="AKD82" s="0"/>
+      <c r="AKE82" s="0"/>
+      <c r="AKF82" s="0"/>
+      <c r="AKG82" s="0"/>
+      <c r="AKH82" s="0"/>
+      <c r="AKI82" s="0"/>
+      <c r="AKJ82" s="0"/>
+      <c r="AKK82" s="0"/>
+      <c r="AKL82" s="0"/>
+      <c r="AKM82" s="0"/>
+      <c r="AKN82" s="0"/>
+      <c r="AKO82" s="0"/>
+      <c r="AKP82" s="0"/>
+      <c r="AKQ82" s="0"/>
+      <c r="AKR82" s="0"/>
+      <c r="AKS82" s="0"/>
+      <c r="AKT82" s="0"/>
+      <c r="AKU82" s="0"/>
+      <c r="AKV82" s="0"/>
+      <c r="AKW82" s="0"/>
+      <c r="AKX82" s="0"/>
+      <c r="AKY82" s="0"/>
+      <c r="AKZ82" s="0"/>
+      <c r="ALA82" s="0"/>
+      <c r="ALB82" s="0"/>
+      <c r="ALC82" s="0"/>
+      <c r="ALD82" s="0"/>
+      <c r="ALE82" s="0"/>
+      <c r="ALF82" s="0"/>
+      <c r="ALG82" s="0"/>
+      <c r="ALH82" s="0"/>
+      <c r="ALI82" s="0"/>
+      <c r="ALJ82" s="0"/>
+      <c r="ALK82" s="0"/>
+      <c r="ALL82" s="0"/>
+      <c r="ALM82" s="0"/>
+      <c r="ALN82" s="0"/>
+      <c r="ALO82" s="0"/>
+      <c r="ALP82" s="0"/>
+      <c r="ALQ82" s="0"/>
+      <c r="ALR82" s="0"/>
+      <c r="ALS82" s="0"/>
+      <c r="ALT82" s="0"/>
+      <c r="ALU82" s="0"/>
+      <c r="ALV82" s="0"/>
+      <c r="ALW82" s="0"/>
+      <c r="ALX82" s="0"/>
+      <c r="ALY82" s="0"/>
+      <c r="ALZ82" s="0"/>
+      <c r="AMA82" s="0"/>
+      <c r="AMB82" s="0"/>
+      <c r="AMC82" s="0"/>
+      <c r="AMD82" s="0"/>
+      <c r="AME82" s="0"/>
+      <c r="AMF82" s="0"/>
+      <c r="AMG82" s="0"/>
+      <c r="AMH82" s="0"/>
+      <c r="AMI82" s="0"/>
+      <c r="AMJ82" s="0"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G68">
@@ -4228,10 +5272,20 @@
     </filterColumn>
     <filterColumn colId="2">
       <customFilters and="true">
-        <customFilter operator="equal" val="Levels"/>
+        <customFilter operator="equal" val="K Distance"/>
       </customFilters>
     </filterColumn>
   </autoFilter>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E1068" type="list">
+      <formula1>"Easy,Medium,Hard"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1068" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="Check for Children Sum Property in a Binary Tree"/>
     <hyperlink ref="A3" r:id="rId2" display="Check sum of Covered and Uncovered nodes of Binary Tree "/>
@@ -4259,8 +5313,8 @@
     <hyperlink ref="A25" r:id="rId24" display="Check if there is a root to leaf path with given sequence "/>
     <hyperlink ref="A26" r:id="rId25" display="Check if a Binary Tree (not BST) has duplicate values "/>
     <hyperlink ref="A27" r:id="rId26" display="Check if removing an edge can divide a Binary Tree in two halves"/>
-    <hyperlink ref="A29" r:id="rId27" display="Print cousins of a given node in Binary Tree"/>
-    <hyperlink ref="A30" r:id="rId28" display="Print cousins of a given node in Binary Tree | Single Traversal"/>
+    <hyperlink ref="A28" r:id="rId27" display="Print cousins of a given node in Binary Tree"/>
+    <hyperlink ref="A29" r:id="rId28" display="Print cousins of a given node in Binary Tree | Single Traversal"/>
     <hyperlink ref="A31" r:id="rId29" display="Print all nodes that don’t have sibling"/>
     <hyperlink ref="A32" r:id="rId30" display="Given a binary tree, print out all of its root-to-leaf paths one per line"/>
     <hyperlink ref="A33" r:id="rId31" display="Print root to leaf paths without using recursion "/>
@@ -4322,12 +5376,12 @@
       <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.28"/>
   </cols>
@@ -4343,7 +5397,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>4</v>
@@ -4357,13 +5411,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>17</v>
@@ -4371,13 +5425,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>17</v>
@@ -4385,13 +5439,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>289</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>17</v>
@@ -4399,13 +5453,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>293</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>290</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>17</v>
@@ -4413,13 +5467,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>17</v>
@@ -4427,13 +5481,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>17</v>
@@ -4441,13 +5495,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>17</v>
@@ -4455,13 +5509,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>17</v>
@@ -4469,13 +5523,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>17</v>
@@ -4483,13 +5537,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>300</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>297</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>17</v>
@@ -4497,10 +5551,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>68</v>
@@ -4511,10 +5565,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>68</v>
@@ -4525,10 +5579,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>68</v>
@@ -4574,13 +5628,13 @@
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="80.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="57.57"/>
@@ -4597,7 +5651,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
@@ -4611,13 +5665,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>17</v>
@@ -4625,13 +5679,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>17</v>
@@ -4639,13 +5693,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>306</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>17</v>
@@ -4653,13 +5707,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>310</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>307</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>17</v>
@@ -4667,13 +5721,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>17</v>
@@ -4681,13 +5735,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>17</v>
@@ -4695,13 +5749,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>17</v>
@@ -4709,13 +5763,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>17</v>
@@ -4723,13 +5777,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>17</v>
@@ -4737,13 +5791,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>317</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>314</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>17</v>
@@ -4751,13 +5805,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>17</v>
@@ -4765,10 +5819,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>203</v>
@@ -4779,10 +5833,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>203</v>
@@ -4793,10 +5847,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>203</v>
@@ -4807,13 +5861,13 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>17</v>
@@ -4821,13 +5875,13 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>17</v>
@@ -4835,13 +5889,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>17</v>
@@ -4849,13 +5903,13 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>326</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>323</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>17</v>
@@ -4863,13 +5917,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>17</v>
@@ -4878,13 +5932,13 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>17</v>
@@ -4892,13 +5946,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>17</v>
@@ -4906,13 +5960,13 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>17</v>
@@ -4920,13 +5974,13 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>17</v>
@@ -4934,10 +5988,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>76</v>
@@ -4948,10 +6002,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>76</v>
@@ -4962,10 +6016,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>76</v>
@@ -4976,10 +6030,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>76</v>
@@ -4990,10 +6044,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>76</v>
@@ -5004,10 +6058,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>76</v>
@@ -5018,10 +6072,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>76</v>
@@ -5032,10 +6086,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>76</v>
@@ -5046,10 +6100,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>76</v>
@@ -5060,10 +6114,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>65</v>
@@ -5074,10 +6128,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>65</v>
@@ -5088,10 +6142,10 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>65</v>
@@ -5102,10 +6156,10 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>65</v>
@@ -5116,10 +6170,10 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>65</v>
@@ -5130,10 +6184,10 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>65</v>
@@ -5144,10 +6198,10 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>65</v>
@@ -5157,16 +6211,16 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12"/>
+      <c r="A41" s="11"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12"/>
+      <c r="A42" s="11"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="12"/>
+      <c r="A50" s="11"/>
     </row>
     <row r="51" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="13"/>
+      <c r="A51" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5231,7 +6285,7 @@
       <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
@@ -5250,7 +6304,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>4</v>
@@ -5267,43 +6321,43 @@
         <v>175</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>348</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -5334,7 +6388,7 @@
       <selection pane="topLeft" activeCell="Q9" activeCellId="0" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="62.29"/>
   </cols>
@@ -5396,11 +6450,11 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.2"/>
@@ -5408,106 +6462,106 @@
   <sheetData>
     <row r="1" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>378</v>
+      <c r="A13" s="13" t="s">
+        <v>381</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BinaryTrees.xls and Added new programs
</commit_message>
<xml_diff>
--- a/resources/BinaryTrees.xlsx
+++ b/resources/BinaryTrees.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="731"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="731" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TraversalAndView" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Tips" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CheckingAndPrinting!$A$1:$G$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CheckingAndPrinting!$A$1:$G$67</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">ConstructionAndConversion!$A$1:$G$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'N-ary Trees'!$A$1:$G$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TraversalAndView!$A$1:$G$47</definedName>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="398">
   <si>
     <t>Name</t>
   </si>
@@ -933,9 +933,6 @@
   </si>
   <si>
     <t>Print odd positioned nodes of even levels in level order of the given binary tree</t>
-  </si>
-  <si>
-    <t>Check whether a given Binary Tree is Complete or not | Set 1 (Iterative Solution)</t>
   </si>
   <si>
     <t>Print middle level of perfect binary tree without finding height</t>
@@ -1331,6 +1328,27 @@
   </si>
   <si>
     <t>printExtremeNodesOfEachLevelInAlternateOrderWithRecursionAndSpiralTraversal</t>
+  </si>
+  <si>
+    <t>printAllFullNodesWithRecursion</t>
+  </si>
+  <si>
+    <t>printAllLeafNodesLeftToRightWithRecursion</t>
+  </si>
+  <si>
+    <t>printNodesAsTheyBecomeLeafNodeWithRecursion</t>
+  </si>
+  <si>
+    <t>printEvenPositionedNodesOfEvenLevelsInLevelOrder</t>
+  </si>
+  <si>
+    <t>printOddPositionedNodesOfOddLevelsInLevelOrder</t>
+  </si>
+  <si>
+    <t>printEvenPositionedNodesOfOddLevelsInLevelOrder</t>
+  </si>
+  <si>
+    <t>printOddPositionedNodesOfEvenLevelsInLevelOrder</t>
   </si>
 </sst>
 </file>
@@ -1774,8 +1792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2678,7 +2696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ53"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -3315,10 +3333,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ1068"/>
+  <dimension ref="A1:AMJ1066"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3328,7 +3346,7 @@
     <col min="3" max="3" width="19.7109375" style="10" customWidth="1"/>
     <col min="4" max="4" width="75.5703125" style="10" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="10"/>
-    <col min="6" max="6" width="10.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="1024" width="9.140625" style="10"/>
   </cols>
   <sheetData>
@@ -4277,8 +4295,14 @@
       <c r="C55" s="1" t="s">
         <v>277</v>
       </c>
+      <c r="D55" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="F55" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -4291,13 +4315,19 @@
       <c r="C56" s="1" t="s">
         <v>277</v>
       </c>
+      <c r="D56" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="F56" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>222</v>
@@ -4305,8 +4335,14 @@
       <c r="C57" s="1" t="s">
         <v>277</v>
       </c>
+      <c r="D57" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="F57" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -4340,7 +4376,7 @@
         <v>280</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E59" s="10" t="s">
         <v>282</v>
@@ -4360,7 +4396,7 @@
         <v>280</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E60" s="10" t="s">
         <v>282</v>
@@ -4380,7 +4416,7 @@
         <v>280</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E61" s="10" t="s">
         <v>282</v>
@@ -4400,7 +4436,7 @@
         <v>280</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>282</v>
@@ -4419,8 +4455,11 @@
       <c r="C63" s="1" t="s">
         <v>288</v>
       </c>
+      <c r="D63" s="10" t="s">
+        <v>394</v>
+      </c>
       <c r="F63" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -4433,11 +4472,14 @@
       <c r="C64" s="1" t="s">
         <v>288</v>
       </c>
+      <c r="D64" s="10" t="s">
+        <v>395</v>
+      </c>
       <c r="F64" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>290</v>
       </c>
@@ -4447,11 +4489,14 @@
       <c r="C65" s="1" t="s">
         <v>288</v>
       </c>
+      <c r="D65" s="10" t="s">
+        <v>396</v>
+      </c>
       <c r="F65" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>291</v>
       </c>
@@ -4461,11 +4506,14 @@
       <c r="C66" s="1" t="s">
         <v>288</v>
       </c>
+      <c r="D66" s="10" t="s">
+        <v>397</v>
+      </c>
       <c r="F66" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>292</v>
       </c>
@@ -4479,1136 +4527,1114 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F80" s="1"/>
-    </row>
-    <row r="81" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A80"/>
+      <c r="B80"/>
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="G80"/>
+      <c r="H80"/>
+      <c r="I80"/>
+      <c r="J80"/>
+      <c r="K80"/>
+      <c r="L80"/>
+      <c r="M80"/>
+      <c r="N80"/>
+      <c r="O80"/>
+      <c r="P80"/>
+      <c r="Q80"/>
+      <c r="R80"/>
+      <c r="S80"/>
+      <c r="T80"/>
+      <c r="U80"/>
+      <c r="V80"/>
+      <c r="W80"/>
+      <c r="X80"/>
+      <c r="Y80"/>
+      <c r="Z80"/>
+      <c r="AA80"/>
+      <c r="AB80"/>
+      <c r="AC80"/>
+      <c r="AD80"/>
+      <c r="AE80"/>
+      <c r="AF80"/>
+      <c r="AG80"/>
+      <c r="AH80"/>
+      <c r="AI80"/>
+      <c r="AJ80"/>
+      <c r="AK80"/>
+      <c r="AL80"/>
+      <c r="AM80"/>
+      <c r="AN80"/>
+      <c r="AO80"/>
+      <c r="AP80"/>
+      <c r="AQ80"/>
+      <c r="AR80"/>
+      <c r="AS80"/>
+      <c r="AT80"/>
+      <c r="AU80"/>
+      <c r="AV80"/>
+      <c r="AW80"/>
+      <c r="AX80"/>
+      <c r="AY80"/>
+      <c r="AZ80"/>
+      <c r="BA80"/>
+      <c r="BB80"/>
+      <c r="BC80"/>
+      <c r="BD80"/>
+      <c r="BE80"/>
+      <c r="BF80"/>
+      <c r="BG80"/>
+      <c r="BH80"/>
+      <c r="BI80"/>
+      <c r="BJ80"/>
+      <c r="BK80"/>
+      <c r="BL80"/>
+      <c r="BM80"/>
+      <c r="BN80"/>
+      <c r="BO80"/>
+      <c r="BP80"/>
+      <c r="BQ80"/>
+      <c r="BR80"/>
+      <c r="BS80"/>
+      <c r="BT80"/>
+      <c r="BU80"/>
+      <c r="BV80"/>
+      <c r="BW80"/>
+      <c r="BX80"/>
+      <c r="BY80"/>
+      <c r="BZ80"/>
+      <c r="CA80"/>
+      <c r="CB80"/>
+      <c r="CC80"/>
+      <c r="CD80"/>
+      <c r="CE80"/>
+      <c r="CF80"/>
+      <c r="CG80"/>
+      <c r="CH80"/>
+      <c r="CI80"/>
+      <c r="CJ80"/>
+      <c r="CK80"/>
+      <c r="CL80"/>
+      <c r="CM80"/>
+      <c r="CN80"/>
+      <c r="CO80"/>
+      <c r="CP80"/>
+      <c r="CQ80"/>
+      <c r="CR80"/>
+      <c r="CS80"/>
+      <c r="CT80"/>
+      <c r="CU80"/>
+      <c r="CV80"/>
+      <c r="CW80"/>
+      <c r="CX80"/>
+      <c r="CY80"/>
+      <c r="CZ80"/>
+      <c r="DA80"/>
+      <c r="DB80"/>
+      <c r="DC80"/>
+      <c r="DD80"/>
+      <c r="DE80"/>
+      <c r="DF80"/>
+      <c r="DG80"/>
+      <c r="DH80"/>
+      <c r="DI80"/>
+      <c r="DJ80"/>
+      <c r="DK80"/>
+      <c r="DL80"/>
+      <c r="DM80"/>
+      <c r="DN80"/>
+      <c r="DO80"/>
+      <c r="DP80"/>
+      <c r="DQ80"/>
+      <c r="DR80"/>
+      <c r="DS80"/>
+      <c r="DT80"/>
+      <c r="DU80"/>
+      <c r="DV80"/>
+      <c r="DW80"/>
+      <c r="DX80"/>
+      <c r="DY80"/>
+      <c r="DZ80"/>
+      <c r="EA80"/>
+      <c r="EB80"/>
+      <c r="EC80"/>
+      <c r="ED80"/>
+      <c r="EE80"/>
+      <c r="EF80"/>
+      <c r="EG80"/>
+      <c r="EH80"/>
+      <c r="EI80"/>
+      <c r="EJ80"/>
+      <c r="EK80"/>
+      <c r="EL80"/>
+      <c r="EM80"/>
+      <c r="EN80"/>
+      <c r="EO80"/>
+      <c r="EP80"/>
+      <c r="EQ80"/>
+      <c r="ER80"/>
+      <c r="ES80"/>
+      <c r="ET80"/>
+      <c r="EU80"/>
+      <c r="EV80"/>
+      <c r="EW80"/>
+      <c r="EX80"/>
+      <c r="EY80"/>
+      <c r="EZ80"/>
+      <c r="FA80"/>
+      <c r="FB80"/>
+      <c r="FC80"/>
+      <c r="FD80"/>
+      <c r="FE80"/>
+      <c r="FF80"/>
+      <c r="FG80"/>
+      <c r="FH80"/>
+      <c r="FI80"/>
+      <c r="FJ80"/>
+      <c r="FK80"/>
+      <c r="FL80"/>
+      <c r="FM80"/>
+      <c r="FN80"/>
+      <c r="FO80"/>
+      <c r="FP80"/>
+      <c r="FQ80"/>
+      <c r="FR80"/>
+      <c r="FS80"/>
+      <c r="FT80"/>
+      <c r="FU80"/>
+      <c r="FV80"/>
+      <c r="FW80"/>
+      <c r="FX80"/>
+      <c r="FY80"/>
+      <c r="FZ80"/>
+      <c r="GA80"/>
+      <c r="GB80"/>
+      <c r="GC80"/>
+      <c r="GD80"/>
+      <c r="GE80"/>
+      <c r="GF80"/>
+      <c r="GG80"/>
+      <c r="GH80"/>
+      <c r="GI80"/>
+      <c r="GJ80"/>
+      <c r="GK80"/>
+      <c r="GL80"/>
+      <c r="GM80"/>
+      <c r="GN80"/>
+      <c r="GO80"/>
+      <c r="GP80"/>
+      <c r="GQ80"/>
+      <c r="GR80"/>
+      <c r="GS80"/>
+      <c r="GT80"/>
+      <c r="GU80"/>
+      <c r="GV80"/>
+      <c r="GW80"/>
+      <c r="GX80"/>
+      <c r="GY80"/>
+      <c r="GZ80"/>
+      <c r="HA80"/>
+      <c r="HB80"/>
+      <c r="HC80"/>
+      <c r="HD80"/>
+      <c r="HE80"/>
+      <c r="HF80"/>
+      <c r="HG80"/>
+      <c r="HH80"/>
+      <c r="HI80"/>
+      <c r="HJ80"/>
+      <c r="HK80"/>
+      <c r="HL80"/>
+      <c r="HM80"/>
+      <c r="HN80"/>
+      <c r="HO80"/>
+      <c r="HP80"/>
+      <c r="HQ80"/>
+      <c r="HR80"/>
+      <c r="HS80"/>
+      <c r="HT80"/>
+      <c r="HU80"/>
+      <c r="HV80"/>
+      <c r="HW80"/>
+      <c r="HX80"/>
+      <c r="HY80"/>
+      <c r="HZ80"/>
+      <c r="IA80"/>
+      <c r="IB80"/>
+      <c r="IC80"/>
+      <c r="ID80"/>
+      <c r="IE80"/>
+      <c r="IF80"/>
+      <c r="IG80"/>
+      <c r="IH80"/>
+      <c r="II80"/>
+      <c r="IJ80"/>
+      <c r="IK80"/>
+      <c r="IL80"/>
+      <c r="IM80"/>
+      <c r="IN80"/>
+      <c r="IO80"/>
+      <c r="IP80"/>
+      <c r="IQ80"/>
+      <c r="IR80"/>
+      <c r="IS80"/>
+      <c r="IT80"/>
+      <c r="IU80"/>
+      <c r="IV80"/>
+      <c r="IW80"/>
+      <c r="IX80"/>
+      <c r="IY80"/>
+      <c r="IZ80"/>
+      <c r="JA80"/>
+      <c r="JB80"/>
+      <c r="JC80"/>
+      <c r="JD80"/>
+      <c r="JE80"/>
+      <c r="JF80"/>
+      <c r="JG80"/>
+      <c r="JH80"/>
+      <c r="JI80"/>
+      <c r="JJ80"/>
+      <c r="JK80"/>
+      <c r="JL80"/>
+      <c r="JM80"/>
+      <c r="JN80"/>
+      <c r="JO80"/>
+      <c r="JP80"/>
+      <c r="JQ80"/>
+      <c r="JR80"/>
+      <c r="JS80"/>
+      <c r="JT80"/>
+      <c r="JU80"/>
+      <c r="JV80"/>
+      <c r="JW80"/>
+      <c r="JX80"/>
+      <c r="JY80"/>
+      <c r="JZ80"/>
+      <c r="KA80"/>
+      <c r="KB80"/>
+      <c r="KC80"/>
+      <c r="KD80"/>
+      <c r="KE80"/>
+      <c r="KF80"/>
+      <c r="KG80"/>
+      <c r="KH80"/>
+      <c r="KI80"/>
+      <c r="KJ80"/>
+      <c r="KK80"/>
+      <c r="KL80"/>
+      <c r="KM80"/>
+      <c r="KN80"/>
+      <c r="KO80"/>
+      <c r="KP80"/>
+      <c r="KQ80"/>
+      <c r="KR80"/>
+      <c r="KS80"/>
+      <c r="KT80"/>
+      <c r="KU80"/>
+      <c r="KV80"/>
+      <c r="KW80"/>
+      <c r="KX80"/>
+      <c r="KY80"/>
+      <c r="KZ80"/>
+      <c r="LA80"/>
+      <c r="LB80"/>
+      <c r="LC80"/>
+      <c r="LD80"/>
+      <c r="LE80"/>
+      <c r="LF80"/>
+      <c r="LG80"/>
+      <c r="LH80"/>
+      <c r="LI80"/>
+      <c r="LJ80"/>
+      <c r="LK80"/>
+      <c r="LL80"/>
+      <c r="LM80"/>
+      <c r="LN80"/>
+      <c r="LO80"/>
+      <c r="LP80"/>
+      <c r="LQ80"/>
+      <c r="LR80"/>
+      <c r="LS80"/>
+      <c r="LT80"/>
+      <c r="LU80"/>
+      <c r="LV80"/>
+      <c r="LW80"/>
+      <c r="LX80"/>
+      <c r="LY80"/>
+      <c r="LZ80"/>
+      <c r="MA80"/>
+      <c r="MB80"/>
+      <c r="MC80"/>
+      <c r="MD80"/>
+      <c r="ME80"/>
+      <c r="MF80"/>
+      <c r="MG80"/>
+      <c r="MH80"/>
+      <c r="MI80"/>
+      <c r="MJ80"/>
+      <c r="MK80"/>
+      <c r="ML80"/>
+      <c r="MM80"/>
+      <c r="MN80"/>
+      <c r="MO80"/>
+      <c r="MP80"/>
+      <c r="MQ80"/>
+      <c r="MR80"/>
+      <c r="MS80"/>
+      <c r="MT80"/>
+      <c r="MU80"/>
+      <c r="MV80"/>
+      <c r="MW80"/>
+      <c r="MX80"/>
+      <c r="MY80"/>
+      <c r="MZ80"/>
+      <c r="NA80"/>
+      <c r="NB80"/>
+      <c r="NC80"/>
+      <c r="ND80"/>
+      <c r="NE80"/>
+      <c r="NF80"/>
+      <c r="NG80"/>
+      <c r="NH80"/>
+      <c r="NI80"/>
+      <c r="NJ80"/>
+      <c r="NK80"/>
+      <c r="NL80"/>
+      <c r="NM80"/>
+      <c r="NN80"/>
+      <c r="NO80"/>
+      <c r="NP80"/>
+      <c r="NQ80"/>
+      <c r="NR80"/>
+      <c r="NS80"/>
+      <c r="NT80"/>
+      <c r="NU80"/>
+      <c r="NV80"/>
+      <c r="NW80"/>
+      <c r="NX80"/>
+      <c r="NY80"/>
+      <c r="NZ80"/>
+      <c r="OA80"/>
+      <c r="OB80"/>
+      <c r="OC80"/>
+      <c r="OD80"/>
+      <c r="OE80"/>
+      <c r="OF80"/>
+      <c r="OG80"/>
+      <c r="OH80"/>
+      <c r="OI80"/>
+      <c r="OJ80"/>
+      <c r="OK80"/>
+      <c r="OL80"/>
+      <c r="OM80"/>
+      <c r="ON80"/>
+      <c r="OO80"/>
+      <c r="OP80"/>
+      <c r="OQ80"/>
+      <c r="OR80"/>
+      <c r="OS80"/>
+      <c r="OT80"/>
+      <c r="OU80"/>
+      <c r="OV80"/>
+      <c r="OW80"/>
+      <c r="OX80"/>
+      <c r="OY80"/>
+      <c r="OZ80"/>
+      <c r="PA80"/>
+      <c r="PB80"/>
+      <c r="PC80"/>
+      <c r="PD80"/>
+      <c r="PE80"/>
+      <c r="PF80"/>
+      <c r="PG80"/>
+      <c r="PH80"/>
+      <c r="PI80"/>
+      <c r="PJ80"/>
+      <c r="PK80"/>
+      <c r="PL80"/>
+      <c r="PM80"/>
+      <c r="PN80"/>
+      <c r="PO80"/>
+      <c r="PP80"/>
+      <c r="PQ80"/>
+      <c r="PR80"/>
+      <c r="PS80"/>
+      <c r="PT80"/>
+      <c r="PU80"/>
+      <c r="PV80"/>
+      <c r="PW80"/>
+      <c r="PX80"/>
+      <c r="PY80"/>
+      <c r="PZ80"/>
+      <c r="QA80"/>
+      <c r="QB80"/>
+      <c r="QC80"/>
+      <c r="QD80"/>
+      <c r="QE80"/>
+      <c r="QF80"/>
+      <c r="QG80"/>
+      <c r="QH80"/>
+      <c r="QI80"/>
+      <c r="QJ80"/>
+      <c r="QK80"/>
+      <c r="QL80"/>
+      <c r="QM80"/>
+      <c r="QN80"/>
+      <c r="QO80"/>
+      <c r="QP80"/>
+      <c r="QQ80"/>
+      <c r="QR80"/>
+      <c r="QS80"/>
+      <c r="QT80"/>
+      <c r="QU80"/>
+      <c r="QV80"/>
+      <c r="QW80"/>
+      <c r="QX80"/>
+      <c r="QY80"/>
+      <c r="QZ80"/>
+      <c r="RA80"/>
+      <c r="RB80"/>
+      <c r="RC80"/>
+      <c r="RD80"/>
+      <c r="RE80"/>
+      <c r="RF80"/>
+      <c r="RG80"/>
+      <c r="RH80"/>
+      <c r="RI80"/>
+      <c r="RJ80"/>
+      <c r="RK80"/>
+      <c r="RL80"/>
+      <c r="RM80"/>
+      <c r="RN80"/>
+      <c r="RO80"/>
+      <c r="RP80"/>
+      <c r="RQ80"/>
+      <c r="RR80"/>
+      <c r="RS80"/>
+      <c r="RT80"/>
+      <c r="RU80"/>
+      <c r="RV80"/>
+      <c r="RW80"/>
+      <c r="RX80"/>
+      <c r="RY80"/>
+      <c r="RZ80"/>
+      <c r="SA80"/>
+      <c r="SB80"/>
+      <c r="SC80"/>
+      <c r="SD80"/>
+      <c r="SE80"/>
+      <c r="SF80"/>
+      <c r="SG80"/>
+      <c r="SH80"/>
+      <c r="SI80"/>
+      <c r="SJ80"/>
+      <c r="SK80"/>
+      <c r="SL80"/>
+      <c r="SM80"/>
+      <c r="SN80"/>
+      <c r="SO80"/>
+      <c r="SP80"/>
+      <c r="SQ80"/>
+      <c r="SR80"/>
+      <c r="SS80"/>
+      <c r="ST80"/>
+      <c r="SU80"/>
+      <c r="SV80"/>
+      <c r="SW80"/>
+      <c r="SX80"/>
+      <c r="SY80"/>
+      <c r="SZ80"/>
+      <c r="TA80"/>
+      <c r="TB80"/>
+      <c r="TC80"/>
+      <c r="TD80"/>
+      <c r="TE80"/>
+      <c r="TF80"/>
+      <c r="TG80"/>
+      <c r="TH80"/>
+      <c r="TI80"/>
+      <c r="TJ80"/>
+      <c r="TK80"/>
+      <c r="TL80"/>
+      <c r="TM80"/>
+      <c r="TN80"/>
+      <c r="TO80"/>
+      <c r="TP80"/>
+      <c r="TQ80"/>
+      <c r="TR80"/>
+      <c r="TS80"/>
+      <c r="TT80"/>
+      <c r="TU80"/>
+      <c r="TV80"/>
+      <c r="TW80"/>
+      <c r="TX80"/>
+      <c r="TY80"/>
+      <c r="TZ80"/>
+      <c r="UA80"/>
+      <c r="UB80"/>
+      <c r="UC80"/>
+      <c r="UD80"/>
+      <c r="UE80"/>
+      <c r="UF80"/>
+      <c r="UG80"/>
+      <c r="UH80"/>
+      <c r="UI80"/>
+      <c r="UJ80"/>
+      <c r="UK80"/>
+      <c r="UL80"/>
+      <c r="UM80"/>
+      <c r="UN80"/>
+      <c r="UO80"/>
+      <c r="UP80"/>
+      <c r="UQ80"/>
+      <c r="UR80"/>
+      <c r="US80"/>
+      <c r="UT80"/>
+      <c r="UU80"/>
+      <c r="UV80"/>
+      <c r="UW80"/>
+      <c r="UX80"/>
+      <c r="UY80"/>
+      <c r="UZ80"/>
+      <c r="VA80"/>
+      <c r="VB80"/>
+      <c r="VC80"/>
+      <c r="VD80"/>
+      <c r="VE80"/>
+      <c r="VF80"/>
+      <c r="VG80"/>
+      <c r="VH80"/>
+      <c r="VI80"/>
+      <c r="VJ80"/>
+      <c r="VK80"/>
+      <c r="VL80"/>
+      <c r="VM80"/>
+      <c r="VN80"/>
+      <c r="VO80"/>
+      <c r="VP80"/>
+      <c r="VQ80"/>
+      <c r="VR80"/>
+      <c r="VS80"/>
+      <c r="VT80"/>
+      <c r="VU80"/>
+      <c r="VV80"/>
+      <c r="VW80"/>
+      <c r="VX80"/>
+      <c r="VY80"/>
+      <c r="VZ80"/>
+      <c r="WA80"/>
+      <c r="WB80"/>
+      <c r="WC80"/>
+      <c r="WD80"/>
+      <c r="WE80"/>
+      <c r="WF80"/>
+      <c r="WG80"/>
+      <c r="WH80"/>
+      <c r="WI80"/>
+      <c r="WJ80"/>
+      <c r="WK80"/>
+      <c r="WL80"/>
+      <c r="WM80"/>
+      <c r="WN80"/>
+      <c r="WO80"/>
+      <c r="WP80"/>
+      <c r="WQ80"/>
+      <c r="WR80"/>
+      <c r="WS80"/>
+      <c r="WT80"/>
+      <c r="WU80"/>
+      <c r="WV80"/>
+      <c r="WW80"/>
+      <c r="WX80"/>
+      <c r="WY80"/>
+      <c r="WZ80"/>
+      <c r="XA80"/>
+      <c r="XB80"/>
+      <c r="XC80"/>
+      <c r="XD80"/>
+      <c r="XE80"/>
+      <c r="XF80"/>
+      <c r="XG80"/>
+      <c r="XH80"/>
+      <c r="XI80"/>
+      <c r="XJ80"/>
+      <c r="XK80"/>
+      <c r="XL80"/>
+      <c r="XM80"/>
+      <c r="XN80"/>
+      <c r="XO80"/>
+      <c r="XP80"/>
+      <c r="XQ80"/>
+      <c r="XR80"/>
+      <c r="XS80"/>
+      <c r="XT80"/>
+      <c r="XU80"/>
+      <c r="XV80"/>
+      <c r="XW80"/>
+      <c r="XX80"/>
+      <c r="XY80"/>
+      <c r="XZ80"/>
+      <c r="YA80"/>
+      <c r="YB80"/>
+      <c r="YC80"/>
+      <c r="YD80"/>
+      <c r="YE80"/>
+      <c r="YF80"/>
+      <c r="YG80"/>
+      <c r="YH80"/>
+      <c r="YI80"/>
+      <c r="YJ80"/>
+      <c r="YK80"/>
+      <c r="YL80"/>
+      <c r="YM80"/>
+      <c r="YN80"/>
+      <c r="YO80"/>
+      <c r="YP80"/>
+      <c r="YQ80"/>
+      <c r="YR80"/>
+      <c r="YS80"/>
+      <c r="YT80"/>
+      <c r="YU80"/>
+      <c r="YV80"/>
+      <c r="YW80"/>
+      <c r="YX80"/>
+      <c r="YY80"/>
+      <c r="YZ80"/>
+      <c r="ZA80"/>
+      <c r="ZB80"/>
+      <c r="ZC80"/>
+      <c r="ZD80"/>
+      <c r="ZE80"/>
+      <c r="ZF80"/>
+      <c r="ZG80"/>
+      <c r="ZH80"/>
+      <c r="ZI80"/>
+      <c r="ZJ80"/>
+      <c r="ZK80"/>
+      <c r="ZL80"/>
+      <c r="ZM80"/>
+      <c r="ZN80"/>
+      <c r="ZO80"/>
+      <c r="ZP80"/>
+      <c r="ZQ80"/>
+      <c r="ZR80"/>
+      <c r="ZS80"/>
+      <c r="ZT80"/>
+      <c r="ZU80"/>
+      <c r="ZV80"/>
+      <c r="ZW80"/>
+      <c r="ZX80"/>
+      <c r="ZY80"/>
+      <c r="ZZ80"/>
+      <c r="AAA80"/>
+      <c r="AAB80"/>
+      <c r="AAC80"/>
+      <c r="AAD80"/>
+      <c r="AAE80"/>
+      <c r="AAF80"/>
+      <c r="AAG80"/>
+      <c r="AAH80"/>
+      <c r="AAI80"/>
+      <c r="AAJ80"/>
+      <c r="AAK80"/>
+      <c r="AAL80"/>
+      <c r="AAM80"/>
+      <c r="AAN80"/>
+      <c r="AAO80"/>
+      <c r="AAP80"/>
+      <c r="AAQ80"/>
+      <c r="AAR80"/>
+      <c r="AAS80"/>
+      <c r="AAT80"/>
+      <c r="AAU80"/>
+      <c r="AAV80"/>
+      <c r="AAW80"/>
+      <c r="AAX80"/>
+      <c r="AAY80"/>
+      <c r="AAZ80"/>
+      <c r="ABA80"/>
+      <c r="ABB80"/>
+      <c r="ABC80"/>
+      <c r="ABD80"/>
+      <c r="ABE80"/>
+      <c r="ABF80"/>
+      <c r="ABG80"/>
+      <c r="ABH80"/>
+      <c r="ABI80"/>
+      <c r="ABJ80"/>
+      <c r="ABK80"/>
+      <c r="ABL80"/>
+      <c r="ABM80"/>
+      <c r="ABN80"/>
+      <c r="ABO80"/>
+      <c r="ABP80"/>
+      <c r="ABQ80"/>
+      <c r="ABR80"/>
+      <c r="ABS80"/>
+      <c r="ABT80"/>
+      <c r="ABU80"/>
+      <c r="ABV80"/>
+      <c r="ABW80"/>
+      <c r="ABX80"/>
+      <c r="ABY80"/>
+      <c r="ABZ80"/>
+      <c r="ACA80"/>
+      <c r="ACB80"/>
+      <c r="ACC80"/>
+      <c r="ACD80"/>
+      <c r="ACE80"/>
+      <c r="ACF80"/>
+      <c r="ACG80"/>
+      <c r="ACH80"/>
+      <c r="ACI80"/>
+      <c r="ACJ80"/>
+      <c r="ACK80"/>
+      <c r="ACL80"/>
+      <c r="ACM80"/>
+      <c r="ACN80"/>
+      <c r="ACO80"/>
+      <c r="ACP80"/>
+      <c r="ACQ80"/>
+      <c r="ACR80"/>
+      <c r="ACS80"/>
+      <c r="ACT80"/>
+      <c r="ACU80"/>
+      <c r="ACV80"/>
+      <c r="ACW80"/>
+      <c r="ACX80"/>
+      <c r="ACY80"/>
+      <c r="ACZ80"/>
+      <c r="ADA80"/>
+      <c r="ADB80"/>
+      <c r="ADC80"/>
+      <c r="ADD80"/>
+      <c r="ADE80"/>
+      <c r="ADF80"/>
+      <c r="ADG80"/>
+      <c r="ADH80"/>
+      <c r="ADI80"/>
+      <c r="ADJ80"/>
+      <c r="ADK80"/>
+      <c r="ADL80"/>
+      <c r="ADM80"/>
+      <c r="ADN80"/>
+      <c r="ADO80"/>
+      <c r="ADP80"/>
+      <c r="ADQ80"/>
+      <c r="ADR80"/>
+      <c r="ADS80"/>
+      <c r="ADT80"/>
+      <c r="ADU80"/>
+      <c r="ADV80"/>
+      <c r="ADW80"/>
+      <c r="ADX80"/>
+      <c r="ADY80"/>
+      <c r="ADZ80"/>
+      <c r="AEA80"/>
+      <c r="AEB80"/>
+      <c r="AEC80"/>
+      <c r="AED80"/>
+      <c r="AEE80"/>
+      <c r="AEF80"/>
+      <c r="AEG80"/>
+      <c r="AEH80"/>
+      <c r="AEI80"/>
+      <c r="AEJ80"/>
+      <c r="AEK80"/>
+      <c r="AEL80"/>
+      <c r="AEM80"/>
+      <c r="AEN80"/>
+      <c r="AEO80"/>
+      <c r="AEP80"/>
+      <c r="AEQ80"/>
+      <c r="AER80"/>
+      <c r="AES80"/>
+      <c r="AET80"/>
+      <c r="AEU80"/>
+      <c r="AEV80"/>
+      <c r="AEW80"/>
+      <c r="AEX80"/>
+      <c r="AEY80"/>
+      <c r="AEZ80"/>
+      <c r="AFA80"/>
+      <c r="AFB80"/>
+      <c r="AFC80"/>
+      <c r="AFD80"/>
+      <c r="AFE80"/>
+      <c r="AFF80"/>
+      <c r="AFG80"/>
+      <c r="AFH80"/>
+      <c r="AFI80"/>
+      <c r="AFJ80"/>
+      <c r="AFK80"/>
+      <c r="AFL80"/>
+      <c r="AFM80"/>
+      <c r="AFN80"/>
+      <c r="AFO80"/>
+      <c r="AFP80"/>
+      <c r="AFQ80"/>
+      <c r="AFR80"/>
+      <c r="AFS80"/>
+      <c r="AFT80"/>
+      <c r="AFU80"/>
+      <c r="AFV80"/>
+      <c r="AFW80"/>
+      <c r="AFX80"/>
+      <c r="AFY80"/>
+      <c r="AFZ80"/>
+      <c r="AGA80"/>
+      <c r="AGB80"/>
+      <c r="AGC80"/>
+      <c r="AGD80"/>
+      <c r="AGE80"/>
+      <c r="AGF80"/>
+      <c r="AGG80"/>
+      <c r="AGH80"/>
+      <c r="AGI80"/>
+      <c r="AGJ80"/>
+      <c r="AGK80"/>
+      <c r="AGL80"/>
+      <c r="AGM80"/>
+      <c r="AGN80"/>
+      <c r="AGO80"/>
+      <c r="AGP80"/>
+      <c r="AGQ80"/>
+      <c r="AGR80"/>
+      <c r="AGS80"/>
+      <c r="AGT80"/>
+      <c r="AGU80"/>
+      <c r="AGV80"/>
+      <c r="AGW80"/>
+      <c r="AGX80"/>
+      <c r="AGY80"/>
+      <c r="AGZ80"/>
+      <c r="AHA80"/>
+      <c r="AHB80"/>
+      <c r="AHC80"/>
+      <c r="AHD80"/>
+      <c r="AHE80"/>
+      <c r="AHF80"/>
+      <c r="AHG80"/>
+      <c r="AHH80"/>
+      <c r="AHI80"/>
+      <c r="AHJ80"/>
+      <c r="AHK80"/>
+      <c r="AHL80"/>
+      <c r="AHM80"/>
+      <c r="AHN80"/>
+      <c r="AHO80"/>
+      <c r="AHP80"/>
+      <c r="AHQ80"/>
+      <c r="AHR80"/>
+      <c r="AHS80"/>
+      <c r="AHT80"/>
+      <c r="AHU80"/>
+      <c r="AHV80"/>
+      <c r="AHW80"/>
+      <c r="AHX80"/>
+      <c r="AHY80"/>
+      <c r="AHZ80"/>
+      <c r="AIA80"/>
+      <c r="AIB80"/>
+      <c r="AIC80"/>
+      <c r="AID80"/>
+      <c r="AIE80"/>
+      <c r="AIF80"/>
+      <c r="AIG80"/>
+      <c r="AIH80"/>
+      <c r="AII80"/>
+      <c r="AIJ80"/>
+      <c r="AIK80"/>
+      <c r="AIL80"/>
+      <c r="AIM80"/>
+      <c r="AIN80"/>
+      <c r="AIO80"/>
+      <c r="AIP80"/>
+      <c r="AIQ80"/>
+      <c r="AIR80"/>
+      <c r="AIS80"/>
+      <c r="AIT80"/>
+      <c r="AIU80"/>
+      <c r="AIV80"/>
+      <c r="AIW80"/>
+      <c r="AIX80"/>
+      <c r="AIY80"/>
+      <c r="AIZ80"/>
+      <c r="AJA80"/>
+      <c r="AJB80"/>
+      <c r="AJC80"/>
+      <c r="AJD80"/>
+      <c r="AJE80"/>
+      <c r="AJF80"/>
+      <c r="AJG80"/>
+      <c r="AJH80"/>
+      <c r="AJI80"/>
+      <c r="AJJ80"/>
+      <c r="AJK80"/>
+      <c r="AJL80"/>
+      <c r="AJM80"/>
+      <c r="AJN80"/>
+      <c r="AJO80"/>
+      <c r="AJP80"/>
+      <c r="AJQ80"/>
+      <c r="AJR80"/>
+      <c r="AJS80"/>
+      <c r="AJT80"/>
+      <c r="AJU80"/>
+      <c r="AJV80"/>
+      <c r="AJW80"/>
+      <c r="AJX80"/>
+      <c r="AJY80"/>
+      <c r="AJZ80"/>
+      <c r="AKA80"/>
+      <c r="AKB80"/>
+      <c r="AKC80"/>
+      <c r="AKD80"/>
+      <c r="AKE80"/>
+      <c r="AKF80"/>
+      <c r="AKG80"/>
+      <c r="AKH80"/>
+      <c r="AKI80"/>
+      <c r="AKJ80"/>
+      <c r="AKK80"/>
+      <c r="AKL80"/>
+      <c r="AKM80"/>
+      <c r="AKN80"/>
+      <c r="AKO80"/>
+      <c r="AKP80"/>
+      <c r="AKQ80"/>
+      <c r="AKR80"/>
+      <c r="AKS80"/>
+      <c r="AKT80"/>
+      <c r="AKU80"/>
+      <c r="AKV80"/>
+      <c r="AKW80"/>
+      <c r="AKX80"/>
+      <c r="AKY80"/>
+      <c r="AKZ80"/>
+      <c r="ALA80"/>
+      <c r="ALB80"/>
+      <c r="ALC80"/>
+      <c r="ALD80"/>
+      <c r="ALE80"/>
+      <c r="ALF80"/>
+      <c r="ALG80"/>
+      <c r="ALH80"/>
+      <c r="ALI80"/>
+      <c r="ALJ80"/>
+      <c r="ALK80"/>
+      <c r="ALL80"/>
+      <c r="ALM80"/>
+      <c r="ALN80"/>
+      <c r="ALO80"/>
+      <c r="ALP80"/>
+      <c r="ALQ80"/>
+      <c r="ALR80"/>
+      <c r="ALS80"/>
+      <c r="ALT80"/>
+      <c r="ALU80"/>
+      <c r="ALV80"/>
+      <c r="ALW80"/>
+      <c r="ALX80"/>
+      <c r="ALY80"/>
+      <c r="ALZ80"/>
+      <c r="AMA80"/>
+      <c r="AMB80"/>
+      <c r="AMC80"/>
+      <c r="AMD80"/>
+      <c r="AME80"/>
+      <c r="AMF80"/>
+      <c r="AMG80"/>
+      <c r="AMH80"/>
+      <c r="AMI80"/>
+      <c r="AMJ80"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="C82"/>
-      <c r="D82"/>
-      <c r="E82"/>
-      <c r="F82"/>
-      <c r="G82"/>
-      <c r="H82"/>
-      <c r="I82"/>
-      <c r="J82"/>
-      <c r="K82"/>
-      <c r="L82"/>
-      <c r="M82"/>
-      <c r="N82"/>
-      <c r="O82"/>
-      <c r="P82"/>
-      <c r="Q82"/>
-      <c r="R82"/>
-      <c r="S82"/>
-      <c r="T82"/>
-      <c r="U82"/>
-      <c r="V82"/>
-      <c r="W82"/>
-      <c r="X82"/>
-      <c r="Y82"/>
-      <c r="Z82"/>
-      <c r="AA82"/>
-      <c r="AB82"/>
-      <c r="AC82"/>
-      <c r="AD82"/>
-      <c r="AE82"/>
-      <c r="AF82"/>
-      <c r="AG82"/>
-      <c r="AH82"/>
-      <c r="AI82"/>
-      <c r="AJ82"/>
-      <c r="AK82"/>
-      <c r="AL82"/>
-      <c r="AM82"/>
-      <c r="AN82"/>
-      <c r="AO82"/>
-      <c r="AP82"/>
-      <c r="AQ82"/>
-      <c r="AR82"/>
-      <c r="AS82"/>
-      <c r="AT82"/>
-      <c r="AU82"/>
-      <c r="AV82"/>
-      <c r="AW82"/>
-      <c r="AX82"/>
-      <c r="AY82"/>
-      <c r="AZ82"/>
-      <c r="BA82"/>
-      <c r="BB82"/>
-      <c r="BC82"/>
-      <c r="BD82"/>
-      <c r="BE82"/>
-      <c r="BF82"/>
-      <c r="BG82"/>
-      <c r="BH82"/>
-      <c r="BI82"/>
-      <c r="BJ82"/>
-      <c r="BK82"/>
-      <c r="BL82"/>
-      <c r="BM82"/>
-      <c r="BN82"/>
-      <c r="BO82"/>
-      <c r="BP82"/>
-      <c r="BQ82"/>
-      <c r="BR82"/>
-      <c r="BS82"/>
-      <c r="BT82"/>
-      <c r="BU82"/>
-      <c r="BV82"/>
-      <c r="BW82"/>
-      <c r="BX82"/>
-      <c r="BY82"/>
-      <c r="BZ82"/>
-      <c r="CA82"/>
-      <c r="CB82"/>
-      <c r="CC82"/>
-      <c r="CD82"/>
-      <c r="CE82"/>
-      <c r="CF82"/>
-      <c r="CG82"/>
-      <c r="CH82"/>
-      <c r="CI82"/>
-      <c r="CJ82"/>
-      <c r="CK82"/>
-      <c r="CL82"/>
-      <c r="CM82"/>
-      <c r="CN82"/>
-      <c r="CO82"/>
-      <c r="CP82"/>
-      <c r="CQ82"/>
-      <c r="CR82"/>
-      <c r="CS82"/>
-      <c r="CT82"/>
-      <c r="CU82"/>
-      <c r="CV82"/>
-      <c r="CW82"/>
-      <c r="CX82"/>
-      <c r="CY82"/>
-      <c r="CZ82"/>
-      <c r="DA82"/>
-      <c r="DB82"/>
-      <c r="DC82"/>
-      <c r="DD82"/>
-      <c r="DE82"/>
-      <c r="DF82"/>
-      <c r="DG82"/>
-      <c r="DH82"/>
-      <c r="DI82"/>
-      <c r="DJ82"/>
-      <c r="DK82"/>
-      <c r="DL82"/>
-      <c r="DM82"/>
-      <c r="DN82"/>
-      <c r="DO82"/>
-      <c r="DP82"/>
-      <c r="DQ82"/>
-      <c r="DR82"/>
-      <c r="DS82"/>
-      <c r="DT82"/>
-      <c r="DU82"/>
-      <c r="DV82"/>
-      <c r="DW82"/>
-      <c r="DX82"/>
-      <c r="DY82"/>
-      <c r="DZ82"/>
-      <c r="EA82"/>
-      <c r="EB82"/>
-      <c r="EC82"/>
-      <c r="ED82"/>
-      <c r="EE82"/>
-      <c r="EF82"/>
-      <c r="EG82"/>
-      <c r="EH82"/>
-      <c r="EI82"/>
-      <c r="EJ82"/>
-      <c r="EK82"/>
-      <c r="EL82"/>
-      <c r="EM82"/>
-      <c r="EN82"/>
-      <c r="EO82"/>
-      <c r="EP82"/>
-      <c r="EQ82"/>
-      <c r="ER82"/>
-      <c r="ES82"/>
-      <c r="ET82"/>
-      <c r="EU82"/>
-      <c r="EV82"/>
-      <c r="EW82"/>
-      <c r="EX82"/>
-      <c r="EY82"/>
-      <c r="EZ82"/>
-      <c r="FA82"/>
-      <c r="FB82"/>
-      <c r="FC82"/>
-      <c r="FD82"/>
-      <c r="FE82"/>
-      <c r="FF82"/>
-      <c r="FG82"/>
-      <c r="FH82"/>
-      <c r="FI82"/>
-      <c r="FJ82"/>
-      <c r="FK82"/>
-      <c r="FL82"/>
-      <c r="FM82"/>
-      <c r="FN82"/>
-      <c r="FO82"/>
-      <c r="FP82"/>
-      <c r="FQ82"/>
-      <c r="FR82"/>
-      <c r="FS82"/>
-      <c r="FT82"/>
-      <c r="FU82"/>
-      <c r="FV82"/>
-      <c r="FW82"/>
-      <c r="FX82"/>
-      <c r="FY82"/>
-      <c r="FZ82"/>
-      <c r="GA82"/>
-      <c r="GB82"/>
-      <c r="GC82"/>
-      <c r="GD82"/>
-      <c r="GE82"/>
-      <c r="GF82"/>
-      <c r="GG82"/>
-      <c r="GH82"/>
-      <c r="GI82"/>
-      <c r="GJ82"/>
-      <c r="GK82"/>
-      <c r="GL82"/>
-      <c r="GM82"/>
-      <c r="GN82"/>
-      <c r="GO82"/>
-      <c r="GP82"/>
-      <c r="GQ82"/>
-      <c r="GR82"/>
-      <c r="GS82"/>
-      <c r="GT82"/>
-      <c r="GU82"/>
-      <c r="GV82"/>
-      <c r="GW82"/>
-      <c r="GX82"/>
-      <c r="GY82"/>
-      <c r="GZ82"/>
-      <c r="HA82"/>
-      <c r="HB82"/>
-      <c r="HC82"/>
-      <c r="HD82"/>
-      <c r="HE82"/>
-      <c r="HF82"/>
-      <c r="HG82"/>
-      <c r="HH82"/>
-      <c r="HI82"/>
-      <c r="HJ82"/>
-      <c r="HK82"/>
-      <c r="HL82"/>
-      <c r="HM82"/>
-      <c r="HN82"/>
-      <c r="HO82"/>
-      <c r="HP82"/>
-      <c r="HQ82"/>
-      <c r="HR82"/>
-      <c r="HS82"/>
-      <c r="HT82"/>
-      <c r="HU82"/>
-      <c r="HV82"/>
-      <c r="HW82"/>
-      <c r="HX82"/>
-      <c r="HY82"/>
-      <c r="HZ82"/>
-      <c r="IA82"/>
-      <c r="IB82"/>
-      <c r="IC82"/>
-      <c r="ID82"/>
-      <c r="IE82"/>
-      <c r="IF82"/>
-      <c r="IG82"/>
-      <c r="IH82"/>
-      <c r="II82"/>
-      <c r="IJ82"/>
-      <c r="IK82"/>
-      <c r="IL82"/>
-      <c r="IM82"/>
-      <c r="IN82"/>
-      <c r="IO82"/>
-      <c r="IP82"/>
-      <c r="IQ82"/>
-      <c r="IR82"/>
-      <c r="IS82"/>
-      <c r="IT82"/>
-      <c r="IU82"/>
-      <c r="IV82"/>
-      <c r="IW82"/>
-      <c r="IX82"/>
-      <c r="IY82"/>
-      <c r="IZ82"/>
-      <c r="JA82"/>
-      <c r="JB82"/>
-      <c r="JC82"/>
-      <c r="JD82"/>
-      <c r="JE82"/>
-      <c r="JF82"/>
-      <c r="JG82"/>
-      <c r="JH82"/>
-      <c r="JI82"/>
-      <c r="JJ82"/>
-      <c r="JK82"/>
-      <c r="JL82"/>
-      <c r="JM82"/>
-      <c r="JN82"/>
-      <c r="JO82"/>
-      <c r="JP82"/>
-      <c r="JQ82"/>
-      <c r="JR82"/>
-      <c r="JS82"/>
-      <c r="JT82"/>
-      <c r="JU82"/>
-      <c r="JV82"/>
-      <c r="JW82"/>
-      <c r="JX82"/>
-      <c r="JY82"/>
-      <c r="JZ82"/>
-      <c r="KA82"/>
-      <c r="KB82"/>
-      <c r="KC82"/>
-      <c r="KD82"/>
-      <c r="KE82"/>
-      <c r="KF82"/>
-      <c r="KG82"/>
-      <c r="KH82"/>
-      <c r="KI82"/>
-      <c r="KJ82"/>
-      <c r="KK82"/>
-      <c r="KL82"/>
-      <c r="KM82"/>
-      <c r="KN82"/>
-      <c r="KO82"/>
-      <c r="KP82"/>
-      <c r="KQ82"/>
-      <c r="KR82"/>
-      <c r="KS82"/>
-      <c r="KT82"/>
-      <c r="KU82"/>
-      <c r="KV82"/>
-      <c r="KW82"/>
-      <c r="KX82"/>
-      <c r="KY82"/>
-      <c r="KZ82"/>
-      <c r="LA82"/>
-      <c r="LB82"/>
-      <c r="LC82"/>
-      <c r="LD82"/>
-      <c r="LE82"/>
-      <c r="LF82"/>
-      <c r="LG82"/>
-      <c r="LH82"/>
-      <c r="LI82"/>
-      <c r="LJ82"/>
-      <c r="LK82"/>
-      <c r="LL82"/>
-      <c r="LM82"/>
-      <c r="LN82"/>
-      <c r="LO82"/>
-      <c r="LP82"/>
-      <c r="LQ82"/>
-      <c r="LR82"/>
-      <c r="LS82"/>
-      <c r="LT82"/>
-      <c r="LU82"/>
-      <c r="LV82"/>
-      <c r="LW82"/>
-      <c r="LX82"/>
-      <c r="LY82"/>
-      <c r="LZ82"/>
-      <c r="MA82"/>
-      <c r="MB82"/>
-      <c r="MC82"/>
-      <c r="MD82"/>
-      <c r="ME82"/>
-      <c r="MF82"/>
-      <c r="MG82"/>
-      <c r="MH82"/>
-      <c r="MI82"/>
-      <c r="MJ82"/>
-      <c r="MK82"/>
-      <c r="ML82"/>
-      <c r="MM82"/>
-      <c r="MN82"/>
-      <c r="MO82"/>
-      <c r="MP82"/>
-      <c r="MQ82"/>
-      <c r="MR82"/>
-      <c r="MS82"/>
-      <c r="MT82"/>
-      <c r="MU82"/>
-      <c r="MV82"/>
-      <c r="MW82"/>
-      <c r="MX82"/>
-      <c r="MY82"/>
-      <c r="MZ82"/>
-      <c r="NA82"/>
-      <c r="NB82"/>
-      <c r="NC82"/>
-      <c r="ND82"/>
-      <c r="NE82"/>
-      <c r="NF82"/>
-      <c r="NG82"/>
-      <c r="NH82"/>
-      <c r="NI82"/>
-      <c r="NJ82"/>
-      <c r="NK82"/>
-      <c r="NL82"/>
-      <c r="NM82"/>
-      <c r="NN82"/>
-      <c r="NO82"/>
-      <c r="NP82"/>
-      <c r="NQ82"/>
-      <c r="NR82"/>
-      <c r="NS82"/>
-      <c r="NT82"/>
-      <c r="NU82"/>
-      <c r="NV82"/>
-      <c r="NW82"/>
-      <c r="NX82"/>
-      <c r="NY82"/>
-      <c r="NZ82"/>
-      <c r="OA82"/>
-      <c r="OB82"/>
-      <c r="OC82"/>
-      <c r="OD82"/>
-      <c r="OE82"/>
-      <c r="OF82"/>
-      <c r="OG82"/>
-      <c r="OH82"/>
-      <c r="OI82"/>
-      <c r="OJ82"/>
-      <c r="OK82"/>
-      <c r="OL82"/>
-      <c r="OM82"/>
-      <c r="ON82"/>
-      <c r="OO82"/>
-      <c r="OP82"/>
-      <c r="OQ82"/>
-      <c r="OR82"/>
-      <c r="OS82"/>
-      <c r="OT82"/>
-      <c r="OU82"/>
-      <c r="OV82"/>
-      <c r="OW82"/>
-      <c r="OX82"/>
-      <c r="OY82"/>
-      <c r="OZ82"/>
-      <c r="PA82"/>
-      <c r="PB82"/>
-      <c r="PC82"/>
-      <c r="PD82"/>
-      <c r="PE82"/>
-      <c r="PF82"/>
-      <c r="PG82"/>
-      <c r="PH82"/>
-      <c r="PI82"/>
-      <c r="PJ82"/>
-      <c r="PK82"/>
-      <c r="PL82"/>
-      <c r="PM82"/>
-      <c r="PN82"/>
-      <c r="PO82"/>
-      <c r="PP82"/>
-      <c r="PQ82"/>
-      <c r="PR82"/>
-      <c r="PS82"/>
-      <c r="PT82"/>
-      <c r="PU82"/>
-      <c r="PV82"/>
-      <c r="PW82"/>
-      <c r="PX82"/>
-      <c r="PY82"/>
-      <c r="PZ82"/>
-      <c r="QA82"/>
-      <c r="QB82"/>
-      <c r="QC82"/>
-      <c r="QD82"/>
-      <c r="QE82"/>
-      <c r="QF82"/>
-      <c r="QG82"/>
-      <c r="QH82"/>
-      <c r="QI82"/>
-      <c r="QJ82"/>
-      <c r="QK82"/>
-      <c r="QL82"/>
-      <c r="QM82"/>
-      <c r="QN82"/>
-      <c r="QO82"/>
-      <c r="QP82"/>
-      <c r="QQ82"/>
-      <c r="QR82"/>
-      <c r="QS82"/>
-      <c r="QT82"/>
-      <c r="QU82"/>
-      <c r="QV82"/>
-      <c r="QW82"/>
-      <c r="QX82"/>
-      <c r="QY82"/>
-      <c r="QZ82"/>
-      <c r="RA82"/>
-      <c r="RB82"/>
-      <c r="RC82"/>
-      <c r="RD82"/>
-      <c r="RE82"/>
-      <c r="RF82"/>
-      <c r="RG82"/>
-      <c r="RH82"/>
-      <c r="RI82"/>
-      <c r="RJ82"/>
-      <c r="RK82"/>
-      <c r="RL82"/>
-      <c r="RM82"/>
-      <c r="RN82"/>
-      <c r="RO82"/>
-      <c r="RP82"/>
-      <c r="RQ82"/>
-      <c r="RR82"/>
-      <c r="RS82"/>
-      <c r="RT82"/>
-      <c r="RU82"/>
-      <c r="RV82"/>
-      <c r="RW82"/>
-      <c r="RX82"/>
-      <c r="RY82"/>
-      <c r="RZ82"/>
-      <c r="SA82"/>
-      <c r="SB82"/>
-      <c r="SC82"/>
-      <c r="SD82"/>
-      <c r="SE82"/>
-      <c r="SF82"/>
-      <c r="SG82"/>
-      <c r="SH82"/>
-      <c r="SI82"/>
-      <c r="SJ82"/>
-      <c r="SK82"/>
-      <c r="SL82"/>
-      <c r="SM82"/>
-      <c r="SN82"/>
-      <c r="SO82"/>
-      <c r="SP82"/>
-      <c r="SQ82"/>
-      <c r="SR82"/>
-      <c r="SS82"/>
-      <c r="ST82"/>
-      <c r="SU82"/>
-      <c r="SV82"/>
-      <c r="SW82"/>
-      <c r="SX82"/>
-      <c r="SY82"/>
-      <c r="SZ82"/>
-      <c r="TA82"/>
-      <c r="TB82"/>
-      <c r="TC82"/>
-      <c r="TD82"/>
-      <c r="TE82"/>
-      <c r="TF82"/>
-      <c r="TG82"/>
-      <c r="TH82"/>
-      <c r="TI82"/>
-      <c r="TJ82"/>
-      <c r="TK82"/>
-      <c r="TL82"/>
-      <c r="TM82"/>
-      <c r="TN82"/>
-      <c r="TO82"/>
-      <c r="TP82"/>
-      <c r="TQ82"/>
-      <c r="TR82"/>
-      <c r="TS82"/>
-      <c r="TT82"/>
-      <c r="TU82"/>
-      <c r="TV82"/>
-      <c r="TW82"/>
-      <c r="TX82"/>
-      <c r="TY82"/>
-      <c r="TZ82"/>
-      <c r="UA82"/>
-      <c r="UB82"/>
-      <c r="UC82"/>
-      <c r="UD82"/>
-      <c r="UE82"/>
-      <c r="UF82"/>
-      <c r="UG82"/>
-      <c r="UH82"/>
-      <c r="UI82"/>
-      <c r="UJ82"/>
-      <c r="UK82"/>
-      <c r="UL82"/>
-      <c r="UM82"/>
-      <c r="UN82"/>
-      <c r="UO82"/>
-      <c r="UP82"/>
-      <c r="UQ82"/>
-      <c r="UR82"/>
-      <c r="US82"/>
-      <c r="UT82"/>
-      <c r="UU82"/>
-      <c r="UV82"/>
-      <c r="UW82"/>
-      <c r="UX82"/>
-      <c r="UY82"/>
-      <c r="UZ82"/>
-      <c r="VA82"/>
-      <c r="VB82"/>
-      <c r="VC82"/>
-      <c r="VD82"/>
-      <c r="VE82"/>
-      <c r="VF82"/>
-      <c r="VG82"/>
-      <c r="VH82"/>
-      <c r="VI82"/>
-      <c r="VJ82"/>
-      <c r="VK82"/>
-      <c r="VL82"/>
-      <c r="VM82"/>
-      <c r="VN82"/>
-      <c r="VO82"/>
-      <c r="VP82"/>
-      <c r="VQ82"/>
-      <c r="VR82"/>
-      <c r="VS82"/>
-      <c r="VT82"/>
-      <c r="VU82"/>
-      <c r="VV82"/>
-      <c r="VW82"/>
-      <c r="VX82"/>
-      <c r="VY82"/>
-      <c r="VZ82"/>
-      <c r="WA82"/>
-      <c r="WB82"/>
-      <c r="WC82"/>
-      <c r="WD82"/>
-      <c r="WE82"/>
-      <c r="WF82"/>
-      <c r="WG82"/>
-      <c r="WH82"/>
-      <c r="WI82"/>
-      <c r="WJ82"/>
-      <c r="WK82"/>
-      <c r="WL82"/>
-      <c r="WM82"/>
-      <c r="WN82"/>
-      <c r="WO82"/>
-      <c r="WP82"/>
-      <c r="WQ82"/>
-      <c r="WR82"/>
-      <c r="WS82"/>
-      <c r="WT82"/>
-      <c r="WU82"/>
-      <c r="WV82"/>
-      <c r="WW82"/>
-      <c r="WX82"/>
-      <c r="WY82"/>
-      <c r="WZ82"/>
-      <c r="XA82"/>
-      <c r="XB82"/>
-      <c r="XC82"/>
-      <c r="XD82"/>
-      <c r="XE82"/>
-      <c r="XF82"/>
-      <c r="XG82"/>
-      <c r="XH82"/>
-      <c r="XI82"/>
-      <c r="XJ82"/>
-      <c r="XK82"/>
-      <c r="XL82"/>
-      <c r="XM82"/>
-      <c r="XN82"/>
-      <c r="XO82"/>
-      <c r="XP82"/>
-      <c r="XQ82"/>
-      <c r="XR82"/>
-      <c r="XS82"/>
-      <c r="XT82"/>
-      <c r="XU82"/>
-      <c r="XV82"/>
-      <c r="XW82"/>
-      <c r="XX82"/>
-      <c r="XY82"/>
-      <c r="XZ82"/>
-      <c r="YA82"/>
-      <c r="YB82"/>
-      <c r="YC82"/>
-      <c r="YD82"/>
-      <c r="YE82"/>
-      <c r="YF82"/>
-      <c r="YG82"/>
-      <c r="YH82"/>
-      <c r="YI82"/>
-      <c r="YJ82"/>
-      <c r="YK82"/>
-      <c r="YL82"/>
-      <c r="YM82"/>
-      <c r="YN82"/>
-      <c r="YO82"/>
-      <c r="YP82"/>
-      <c r="YQ82"/>
-      <c r="YR82"/>
-      <c r="YS82"/>
-      <c r="YT82"/>
-      <c r="YU82"/>
-      <c r="YV82"/>
-      <c r="YW82"/>
-      <c r="YX82"/>
-      <c r="YY82"/>
-      <c r="YZ82"/>
-      <c r="ZA82"/>
-      <c r="ZB82"/>
-      <c r="ZC82"/>
-      <c r="ZD82"/>
-      <c r="ZE82"/>
-      <c r="ZF82"/>
-      <c r="ZG82"/>
-      <c r="ZH82"/>
-      <c r="ZI82"/>
-      <c r="ZJ82"/>
-      <c r="ZK82"/>
-      <c r="ZL82"/>
-      <c r="ZM82"/>
-      <c r="ZN82"/>
-      <c r="ZO82"/>
-      <c r="ZP82"/>
-      <c r="ZQ82"/>
-      <c r="ZR82"/>
-      <c r="ZS82"/>
-      <c r="ZT82"/>
-      <c r="ZU82"/>
-      <c r="ZV82"/>
-      <c r="ZW82"/>
-      <c r="ZX82"/>
-      <c r="ZY82"/>
-      <c r="ZZ82"/>
-      <c r="AAA82"/>
-      <c r="AAB82"/>
-      <c r="AAC82"/>
-      <c r="AAD82"/>
-      <c r="AAE82"/>
-      <c r="AAF82"/>
-      <c r="AAG82"/>
-      <c r="AAH82"/>
-      <c r="AAI82"/>
-      <c r="AAJ82"/>
-      <c r="AAK82"/>
-      <c r="AAL82"/>
-      <c r="AAM82"/>
-      <c r="AAN82"/>
-      <c r="AAO82"/>
-      <c r="AAP82"/>
-      <c r="AAQ82"/>
-      <c r="AAR82"/>
-      <c r="AAS82"/>
-      <c r="AAT82"/>
-      <c r="AAU82"/>
-      <c r="AAV82"/>
-      <c r="AAW82"/>
-      <c r="AAX82"/>
-      <c r="AAY82"/>
-      <c r="AAZ82"/>
-      <c r="ABA82"/>
-      <c r="ABB82"/>
-      <c r="ABC82"/>
-      <c r="ABD82"/>
-      <c r="ABE82"/>
-      <c r="ABF82"/>
-      <c r="ABG82"/>
-      <c r="ABH82"/>
-      <c r="ABI82"/>
-      <c r="ABJ82"/>
-      <c r="ABK82"/>
-      <c r="ABL82"/>
-      <c r="ABM82"/>
-      <c r="ABN82"/>
-      <c r="ABO82"/>
-      <c r="ABP82"/>
-      <c r="ABQ82"/>
-      <c r="ABR82"/>
-      <c r="ABS82"/>
-      <c r="ABT82"/>
-      <c r="ABU82"/>
-      <c r="ABV82"/>
-      <c r="ABW82"/>
-      <c r="ABX82"/>
-      <c r="ABY82"/>
-      <c r="ABZ82"/>
-      <c r="ACA82"/>
-      <c r="ACB82"/>
-      <c r="ACC82"/>
-      <c r="ACD82"/>
-      <c r="ACE82"/>
-      <c r="ACF82"/>
-      <c r="ACG82"/>
-      <c r="ACH82"/>
-      <c r="ACI82"/>
-      <c r="ACJ82"/>
-      <c r="ACK82"/>
-      <c r="ACL82"/>
-      <c r="ACM82"/>
-      <c r="ACN82"/>
-      <c r="ACO82"/>
-      <c r="ACP82"/>
-      <c r="ACQ82"/>
-      <c r="ACR82"/>
-      <c r="ACS82"/>
-      <c r="ACT82"/>
-      <c r="ACU82"/>
-      <c r="ACV82"/>
-      <c r="ACW82"/>
-      <c r="ACX82"/>
-      <c r="ACY82"/>
-      <c r="ACZ82"/>
-      <c r="ADA82"/>
-      <c r="ADB82"/>
-      <c r="ADC82"/>
-      <c r="ADD82"/>
-      <c r="ADE82"/>
-      <c r="ADF82"/>
-      <c r="ADG82"/>
-      <c r="ADH82"/>
-      <c r="ADI82"/>
-      <c r="ADJ82"/>
-      <c r="ADK82"/>
-      <c r="ADL82"/>
-      <c r="ADM82"/>
-      <c r="ADN82"/>
-      <c r="ADO82"/>
-      <c r="ADP82"/>
-      <c r="ADQ82"/>
-      <c r="ADR82"/>
-      <c r="ADS82"/>
-      <c r="ADT82"/>
-      <c r="ADU82"/>
-      <c r="ADV82"/>
-      <c r="ADW82"/>
-      <c r="ADX82"/>
-      <c r="ADY82"/>
-      <c r="ADZ82"/>
-      <c r="AEA82"/>
-      <c r="AEB82"/>
-      <c r="AEC82"/>
-      <c r="AED82"/>
-      <c r="AEE82"/>
-      <c r="AEF82"/>
-      <c r="AEG82"/>
-      <c r="AEH82"/>
-      <c r="AEI82"/>
-      <c r="AEJ82"/>
-      <c r="AEK82"/>
-      <c r="AEL82"/>
-      <c r="AEM82"/>
-      <c r="AEN82"/>
-      <c r="AEO82"/>
-      <c r="AEP82"/>
-      <c r="AEQ82"/>
-      <c r="AER82"/>
-      <c r="AES82"/>
-      <c r="AET82"/>
-      <c r="AEU82"/>
-      <c r="AEV82"/>
-      <c r="AEW82"/>
-      <c r="AEX82"/>
-      <c r="AEY82"/>
-      <c r="AEZ82"/>
-      <c r="AFA82"/>
-      <c r="AFB82"/>
-      <c r="AFC82"/>
-      <c r="AFD82"/>
-      <c r="AFE82"/>
-      <c r="AFF82"/>
-      <c r="AFG82"/>
-      <c r="AFH82"/>
-      <c r="AFI82"/>
-      <c r="AFJ82"/>
-      <c r="AFK82"/>
-      <c r="AFL82"/>
-      <c r="AFM82"/>
-      <c r="AFN82"/>
-      <c r="AFO82"/>
-      <c r="AFP82"/>
-      <c r="AFQ82"/>
-      <c r="AFR82"/>
-      <c r="AFS82"/>
-      <c r="AFT82"/>
-      <c r="AFU82"/>
-      <c r="AFV82"/>
-      <c r="AFW82"/>
-      <c r="AFX82"/>
-      <c r="AFY82"/>
-      <c r="AFZ82"/>
-      <c r="AGA82"/>
-      <c r="AGB82"/>
-      <c r="AGC82"/>
-      <c r="AGD82"/>
-      <c r="AGE82"/>
-      <c r="AGF82"/>
-      <c r="AGG82"/>
-      <c r="AGH82"/>
-      <c r="AGI82"/>
-      <c r="AGJ82"/>
-      <c r="AGK82"/>
-      <c r="AGL82"/>
-      <c r="AGM82"/>
-      <c r="AGN82"/>
-      <c r="AGO82"/>
-      <c r="AGP82"/>
-      <c r="AGQ82"/>
-      <c r="AGR82"/>
-      <c r="AGS82"/>
-      <c r="AGT82"/>
-      <c r="AGU82"/>
-      <c r="AGV82"/>
-      <c r="AGW82"/>
-      <c r="AGX82"/>
-      <c r="AGY82"/>
-      <c r="AGZ82"/>
-      <c r="AHA82"/>
-      <c r="AHB82"/>
-      <c r="AHC82"/>
-      <c r="AHD82"/>
-      <c r="AHE82"/>
-      <c r="AHF82"/>
-      <c r="AHG82"/>
-      <c r="AHH82"/>
-      <c r="AHI82"/>
-      <c r="AHJ82"/>
-      <c r="AHK82"/>
-      <c r="AHL82"/>
-      <c r="AHM82"/>
-      <c r="AHN82"/>
-      <c r="AHO82"/>
-      <c r="AHP82"/>
-      <c r="AHQ82"/>
-      <c r="AHR82"/>
-      <c r="AHS82"/>
-      <c r="AHT82"/>
-      <c r="AHU82"/>
-      <c r="AHV82"/>
-      <c r="AHW82"/>
-      <c r="AHX82"/>
-      <c r="AHY82"/>
-      <c r="AHZ82"/>
-      <c r="AIA82"/>
-      <c r="AIB82"/>
-      <c r="AIC82"/>
-      <c r="AID82"/>
-      <c r="AIE82"/>
-      <c r="AIF82"/>
-      <c r="AIG82"/>
-      <c r="AIH82"/>
-      <c r="AII82"/>
-      <c r="AIJ82"/>
-      <c r="AIK82"/>
-      <c r="AIL82"/>
-      <c r="AIM82"/>
-      <c r="AIN82"/>
-      <c r="AIO82"/>
-      <c r="AIP82"/>
-      <c r="AIQ82"/>
-      <c r="AIR82"/>
-      <c r="AIS82"/>
-      <c r="AIT82"/>
-      <c r="AIU82"/>
-      <c r="AIV82"/>
-      <c r="AIW82"/>
-      <c r="AIX82"/>
-      <c r="AIY82"/>
-      <c r="AIZ82"/>
-      <c r="AJA82"/>
-      <c r="AJB82"/>
-      <c r="AJC82"/>
-      <c r="AJD82"/>
-      <c r="AJE82"/>
-      <c r="AJF82"/>
-      <c r="AJG82"/>
-      <c r="AJH82"/>
-      <c r="AJI82"/>
-      <c r="AJJ82"/>
-      <c r="AJK82"/>
-      <c r="AJL82"/>
-      <c r="AJM82"/>
-      <c r="AJN82"/>
-      <c r="AJO82"/>
-      <c r="AJP82"/>
-      <c r="AJQ82"/>
-      <c r="AJR82"/>
-      <c r="AJS82"/>
-      <c r="AJT82"/>
-      <c r="AJU82"/>
-      <c r="AJV82"/>
-      <c r="AJW82"/>
-      <c r="AJX82"/>
-      <c r="AJY82"/>
-      <c r="AJZ82"/>
-      <c r="AKA82"/>
-      <c r="AKB82"/>
-      <c r="AKC82"/>
-      <c r="AKD82"/>
-      <c r="AKE82"/>
-      <c r="AKF82"/>
-      <c r="AKG82"/>
-      <c r="AKH82"/>
-      <c r="AKI82"/>
-      <c r="AKJ82"/>
-      <c r="AKK82"/>
-      <c r="AKL82"/>
-      <c r="AKM82"/>
-      <c r="AKN82"/>
-      <c r="AKO82"/>
-      <c r="AKP82"/>
-      <c r="AKQ82"/>
-      <c r="AKR82"/>
-      <c r="AKS82"/>
-      <c r="AKT82"/>
-      <c r="AKU82"/>
-      <c r="AKV82"/>
-      <c r="AKW82"/>
-      <c r="AKX82"/>
-      <c r="AKY82"/>
-      <c r="AKZ82"/>
-      <c r="ALA82"/>
-      <c r="ALB82"/>
-      <c r="ALC82"/>
-      <c r="ALD82"/>
-      <c r="ALE82"/>
-      <c r="ALF82"/>
-      <c r="ALG82"/>
-      <c r="ALH82"/>
-      <c r="ALI82"/>
-      <c r="ALJ82"/>
-      <c r="ALK82"/>
-      <c r="ALL82"/>
-      <c r="ALM82"/>
-      <c r="ALN82"/>
-      <c r="ALO82"/>
-      <c r="ALP82"/>
-      <c r="ALQ82"/>
-      <c r="ALR82"/>
-      <c r="ALS82"/>
-      <c r="ALT82"/>
-      <c r="ALU82"/>
-      <c r="ALV82"/>
-      <c r="ALW82"/>
-      <c r="ALX82"/>
-      <c r="ALY82"/>
-      <c r="ALZ82"/>
-      <c r="AMA82"/>
-      <c r="AMB82"/>
-      <c r="AMC82"/>
-      <c r="AMD82"/>
-      <c r="AME82"/>
-      <c r="AMF82"/>
-      <c r="AMG82"/>
-      <c r="AMH82"/>
-      <c r="AMI82"/>
-      <c r="AMJ82"/>
-    </row>
-    <row r="83" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="1"/>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F96" s="1"/>
     </row>
     <row r="97" spans="6:6" x14ac:dyDescent="0.25">
@@ -8521,19 +8547,13 @@
     <row r="1066" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1066" s="1"/>
     </row>
-    <row r="1067" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1067" s="1"/>
-    </row>
-    <row r="1068" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1068" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E2:E1068">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="E2:E1066">
       <formula1>"Easy,Medium,Hard"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="F2:F1068">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="F2:F1066">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8603,12 +8623,10 @@
     <hyperlink ref="A65" r:id="rId62"/>
     <hyperlink ref="A66" r:id="rId63"/>
     <hyperlink ref="A67" r:id="rId64"/>
-    <hyperlink ref="A68" r:id="rId65"/>
-    <hyperlink ref="A69" r:id="rId66"/>
-    <hyperlink ref="A57" r:id="rId67"/>
+    <hyperlink ref="A57" r:id="rId65"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId68"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId66"/>
 </worksheet>
 </file>
 
@@ -8616,7 +8634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -8641,7 +8659,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>4</v>
@@ -8655,13 +8673,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" t="s">
         <v>295</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>296</v>
-      </c>
-      <c r="C2" t="s">
-        <v>297</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -8669,13 +8687,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" t="s">
         <v>296</v>
-      </c>
-      <c r="C3" t="s">
-        <v>297</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -8683,13 +8701,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" t="s">
         <v>296</v>
-      </c>
-      <c r="C4" t="s">
-        <v>297</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -8697,13 +8715,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" t="s">
         <v>296</v>
-      </c>
-      <c r="C5" t="s">
-        <v>297</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -8711,13 +8729,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C6" t="s">
         <v>296</v>
-      </c>
-      <c r="C6" t="s">
-        <v>297</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -8725,13 +8743,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C7" t="s">
         <v>296</v>
-      </c>
-      <c r="C7" t="s">
-        <v>297</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -8739,13 +8757,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="B8" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" t="s">
         <v>303</v>
-      </c>
-      <c r="B8" t="s">
-        <v>296</v>
-      </c>
-      <c r="C8" t="s">
-        <v>304</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -8753,13 +8771,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
@@ -8767,13 +8785,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
@@ -8781,13 +8799,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -8795,10 +8813,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C12" t="s">
         <v>68</v>
@@ -8809,10 +8827,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C13" t="s">
         <v>68</v>
@@ -8823,10 +8841,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C14" t="s">
         <v>68</v>
@@ -8887,7 +8905,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
@@ -8901,13 +8919,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" t="s">
         <v>312</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>313</v>
-      </c>
-      <c r="C2" t="s">
-        <v>314</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -8915,13 +8933,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" t="s">
         <v>313</v>
-      </c>
-      <c r="C3" t="s">
-        <v>314</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -8929,13 +8947,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C4" t="s">
         <v>313</v>
-      </c>
-      <c r="C4" t="s">
-        <v>314</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -8943,13 +8961,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5" t="s">
         <v>313</v>
-      </c>
-      <c r="C5" t="s">
-        <v>314</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -8957,13 +8975,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C6" t="s">
         <v>313</v>
-      </c>
-      <c r="C6" t="s">
-        <v>314</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -8971,13 +8989,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" t="s">
         <v>313</v>
-      </c>
-      <c r="C7" t="s">
-        <v>314</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -8985,13 +9003,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="B8" t="s">
+        <v>312</v>
+      </c>
+      <c r="C8" t="s">
         <v>320</v>
-      </c>
-      <c r="B8" t="s">
-        <v>313</v>
-      </c>
-      <c r="C8" t="s">
-        <v>321</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -8999,13 +9017,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
@@ -9013,13 +9031,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
@@ -9027,13 +9045,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -9041,13 +9059,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -9055,10 +9073,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C13" t="s">
         <v>203</v>
@@ -9069,10 +9087,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C14" t="s">
         <v>203</v>
@@ -9083,10 +9101,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C15" t="s">
         <v>203</v>
@@ -9097,13 +9115,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="B16" t="s">
+        <v>312</v>
+      </c>
+      <c r="C16" t="s">
         <v>329</v>
-      </c>
-      <c r="B16" t="s">
-        <v>313</v>
-      </c>
-      <c r="C16" t="s">
-        <v>330</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -9111,13 +9129,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
@@ -9125,13 +9143,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F18" t="s">
         <v>17</v>
@@ -9139,13 +9157,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -9153,13 +9171,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F20" t="s">
         <v>17</v>
@@ -9168,13 +9186,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -9182,13 +9200,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C22" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F22" t="s">
         <v>17</v>
@@ -9196,13 +9214,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
@@ -9210,13 +9228,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F24" t="s">
         <v>17</v>
@@ -9224,10 +9242,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C25" t="s">
         <v>76</v>
@@ -9238,10 +9256,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C26" t="s">
         <v>76</v>
@@ -9252,10 +9270,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C27" t="s">
         <v>76</v>
@@ -9266,10 +9284,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C28" t="s">
         <v>76</v>
@@ -9280,10 +9298,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C29" t="s">
         <v>76</v>
@@ -9294,10 +9312,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C30" t="s">
         <v>76</v>
@@ -9308,10 +9326,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C31" t="s">
         <v>76</v>
@@ -9322,10 +9340,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B32" t="s">
         <v>312</v>
-      </c>
-      <c r="B32" t="s">
-        <v>313</v>
       </c>
       <c r="C32" t="s">
         <v>76</v>
@@ -9336,10 +9354,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B33" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C33" t="s">
         <v>76</v>
@@ -9350,10 +9368,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C34" t="s">
         <v>65</v>
@@ -9364,10 +9382,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B35" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C35" t="s">
         <v>65</v>
@@ -9378,10 +9396,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C36" t="s">
         <v>65</v>
@@ -9392,10 +9410,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B37" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C37" t="s">
         <v>65</v>
@@ -9406,10 +9424,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C38" t="s">
         <v>65</v>
@@ -9420,10 +9438,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B39" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C39" t="s">
         <v>65</v>
@@ -9434,10 +9452,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B40" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C40" t="s">
         <v>65</v>
@@ -9532,7 +9550,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>4</v>
@@ -9549,43 +9567,43 @@
         <v>175</v>
       </c>
       <c r="B2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C2" t="s">
         <v>355</v>
-      </c>
-      <c r="C2" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="B4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C4" t="s">
         <v>358</v>
-      </c>
-      <c r="B4" t="s">
-        <v>355</v>
-      </c>
-      <c r="C4" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="B5" t="s">
+        <v>354</v>
+      </c>
+      <c r="C5" t="s">
         <v>360</v>
-      </c>
-      <c r="B5" t="s">
-        <v>355</v>
-      </c>
-      <c r="C5" t="s">
-        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -9674,106 +9692,106 @@
   <sheetData>
     <row r="1" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>362</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>368</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>383</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="B13" t="s">
         <v>385</v>
-      </c>
-      <c r="B13" t="s">
-        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BinaryTrees.xls and Added new programs in CheckingAndPrinting
</commit_message>
<xml_diff>
--- a/resources/BinaryTrees.xlsx
+++ b/resources/BinaryTrees.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="731" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="731"/>
   </bookViews>
   <sheets>
     <sheet name="TraversalAndView" sheetId="1" r:id="rId1"/>
@@ -23,21 +23,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CheckingAndPrinting!$A$1:$G$67</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">ConstructionAndConversion!$A$1:$G$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ConstructionAndConversion!$A$1:$G$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'N-ary Trees'!$A$1:$G$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TraversalAndView!$A$1:$G$47</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="496">
   <si>
     <t>Name</t>
   </si>
@@ -1613,6 +1608,36 @@
   </si>
   <si>
     <t>85. Minimum no. of iterations to pass information to all nodes in the tree</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>printLengthOfRootToLeafPathWithMaximumDistinctNodes</t>
+  </si>
+  <si>
+    <t>removeNodesOnRootToLeafPathsOfLengthLessThanK</t>
+  </si>
+  <si>
+    <t>Parent and Child is well defined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreOrder must handle null values too </t>
+  </si>
+  <si>
+    <t>checkIfOneTreeIsSubtreeOfAnotherTreeWithoutRecursionWithPreOrderUtil</t>
+  </si>
+  <si>
+    <t>checkIfTwoNodesAreInSameSubtreeOfTheRootNodeWithRecursionAndSet</t>
+  </si>
+  <si>
+    <t>If both in left subtree or both in right subtree, then Yes. Else No</t>
+  </si>
+  <si>
+    <t>Each subtree means from that node till the leaves, not some nodes in themiddle</t>
+  </si>
+  <si>
+    <t>checkIfBinaryTreeContainsDuplicateSubtreesOfSizeTwoOrMoreWithRecursion</t>
   </si>
 </sst>
 </file>
@@ -2056,8 +2081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2961,7 +2986,7 @@
   <dimension ref="A1:AMJ53"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="68.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3600,13 +3625,13 @@
   <dimension ref="A1:AMJ1066"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="81.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="10" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" style="10" customWidth="1"/>
     <col min="4" max="4" width="75.5703125" style="10" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="10"/>
@@ -3908,7 +3933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>200</v>
       </c>
@@ -3925,7 +3950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>202</v>
       </c>
@@ -3938,11 +3963,17 @@
       <c r="D18" s="10" t="s">
         <v>204</v>
       </c>
+      <c r="E18" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>205</v>
       </c>
@@ -3959,7 +3990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>207</v>
       </c>
@@ -3969,11 +4000,17 @@
       <c r="C20" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="D20" s="10" t="s">
+        <v>491</v>
+      </c>
       <c r="F20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>208</v>
       </c>
@@ -3983,11 +4020,20 @@
       <c r="C21" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="D21" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>282</v>
+      </c>
       <c r="F21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>209</v>
       </c>
@@ -3997,11 +4043,20 @@
       <c r="C22" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="D22" s="10" t="s">
+        <v>495</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="F22" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>210</v>
       </c>
@@ -4018,7 +4073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>212</v>
       </c>
@@ -4035,7 +4090,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>214</v>
       </c>
@@ -4052,7 +4107,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>217</v>
       </c>
@@ -4069,7 +4124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>219</v>
       </c>
@@ -4086,7 +4141,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>221</v>
       </c>
@@ -4103,7 +4158,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>224</v>
       </c>
@@ -4120,7 +4175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>226</v>
       </c>
@@ -4137,7 +4192,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>228</v>
       </c>
@@ -4154,7 +4209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>230</v>
       </c>
@@ -4215,8 +4270,14 @@
       <c r="C35" s="1" t="s">
         <v>215</v>
       </c>
+      <c r="D35" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="F35" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -4229,8 +4290,14 @@
       <c r="C36" s="1" t="s">
         <v>215</v>
       </c>
+      <c r="D36" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="F36" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -8908,7 +8975,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8988,7 +9055,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="B5" t="s">
         <v>295</v>
@@ -9002,7 +9069,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B6" t="s">
         <v>295</v>
@@ -9016,7 +9083,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B7" t="s">
         <v>295</v>
@@ -9030,13 +9097,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B8" t="s">
         <v>295</v>
       </c>
       <c r="C8" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -9044,7 +9111,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B9" t="s">
         <v>295</v>
@@ -9058,7 +9125,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B10" t="s">
         <v>295</v>
@@ -9072,7 +9139,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B11" t="s">
         <v>295</v>
@@ -9086,13 +9153,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B12" t="s">
         <v>295</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>303</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -9100,7 +9167,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B13" t="s">
         <v>295</v>
@@ -9114,7 +9181,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B14" t="s">
         <v>295</v>
@@ -9131,16 +9198,16 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
-    <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="A8" r:id="rId6"/>
+    <hyperlink ref="A9" r:id="rId7"/>
+    <hyperlink ref="A10" r:id="rId8"/>
+    <hyperlink ref="A11" r:id="rId9"/>
+    <hyperlink ref="A12" r:id="rId10"/>
+    <hyperlink ref="A13" r:id="rId11"/>
+    <hyperlink ref="A14" r:id="rId12"/>
+    <hyperlink ref="A5" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9152,7 +9219,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="A2:B40"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9895,8 +9962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10426,9 +10493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Updated BinaryTrees.xls and Added LowestCommonAncestor.java
</commit_message>
<xml_diff>
--- a/resources/BinaryTrees.xlsx
+++ b/resources/BinaryTrees.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="731"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="643" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TraversalAndView" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="509">
   <si>
     <t>Name</t>
   </si>
@@ -955,9 +955,6 @@
   </si>
   <si>
     <t>Print Ancestors of a given node in Binary Tree</t>
-  </si>
-  <si>
-    <t>Kth ancestor of a node in binary tree</t>
   </si>
   <si>
     <t>Print the path common to the two paths from the root to the two given nodes</t>
@@ -1638,6 +1635,54 @@
   </si>
   <si>
     <t>checkIfBinaryTreeContainsDuplicateSubtreesOfSizeTwoOrMoreWithRecursion</t>
+  </si>
+  <si>
+    <t>findLowestCommonAncestorWithRootToNodePathComparison
+findLowestCommonAncestorWithRecursion</t>
+  </si>
+  <si>
+    <t>Last common node in Root To Node paths for each value
+If node.data == num1 || num2, return node. Recursively call for left and right subtree.
+If left != null and right != null, return node. Else return whichever is non null</t>
+  </si>
+  <si>
+    <t>findLowestCommonAncestorWithParentPointer</t>
+  </si>
+  <si>
+    <t>On Hold due to RMQ</t>
+  </si>
+  <si>
+    <t>printAncestorsOfGivenNodeWithRecursionAndExtraArray
+printAncestorsOfGivenNodeWithRecursionWithoutExtraArray</t>
+  </si>
+  <si>
+    <t>K-th ancestor of a node in Binary Tree</t>
+  </si>
+  <si>
+    <t>Kth ancestor of a node in binary tree | Set 2</t>
+  </si>
+  <si>
+    <t>Root to Node path without last node</t>
+  </si>
+  <si>
+    <t>Save all parent pointers of first node. First parent pointer of second node to match that of the first node is LCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">printKthAncestorOfANodeInBinaryTreeWithRecursionAndExtraArray
+printKthAncestorOfANodeInBinaryTreeWithRecursionWithoutExtraArray
+</t>
+  </si>
+  <si>
+    <t>printKthAncestorOfANodeInBinaryTreeWithoutRecursionWithStack</t>
+  </si>
+  <si>
+    <t>printAncestorsOfGivenNodeWithoutRecursionWithStack</t>
+  </si>
+  <si>
+    <t>DFS using Stack</t>
+  </si>
+  <si>
+    <t>Root to Node path : arr[last level - k]</t>
   </si>
 </sst>
 </file>
@@ -1698,7 +1743,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1730,6 +1775,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2081,7 +2130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -3625,7 +3674,7 @@
   <dimension ref="A1:AMJ1066"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3970,7 +4019,7 @@
         <v>11</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -4001,13 +4050,13 @@
         <v>203</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -4021,7 +4070,7 @@
         <v>203</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>282</v>
@@ -4030,7 +4079,7 @@
         <v>11</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -4044,16 +4093,16 @@
         <v>203</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -4271,10 +4320,10 @@
         <v>215</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>11</v>
@@ -4291,10 +4340,10 @@
         <v>215</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>11</v>
@@ -4328,13 +4377,13 @@
         <v>215</v>
       </c>
       <c r="D38" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4633,7 +4682,7 @@
         <v>277</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E55" s="10" t="s">
         <v>282</v>
@@ -4653,7 +4702,7 @@
         <v>277</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>282</v>
@@ -4664,7 +4713,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>222</v>
@@ -4673,7 +4722,7 @@
         <v>277</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E57" s="10" t="s">
         <v>282</v>
@@ -4713,7 +4762,7 @@
         <v>280</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E59" s="10" t="s">
         <v>282</v>
@@ -4733,7 +4782,7 @@
         <v>280</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E60" s="10" t="s">
         <v>282</v>
@@ -4753,7 +4802,7 @@
         <v>280</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E61" s="10" t="s">
         <v>282</v>
@@ -4773,7 +4822,7 @@
         <v>280</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>282</v>
@@ -4793,7 +4842,7 @@
         <v>288</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>11</v>
@@ -4810,7 +4859,7 @@
         <v>288</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>11</v>
@@ -4827,7 +4876,7 @@
         <v>288</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>11</v>
@@ -4844,7 +4893,7 @@
         <v>288</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>11</v>
@@ -4861,7 +4910,7 @@
         <v>178</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>11</v>
@@ -8972,20 +9021,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="71.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="63.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -9011,206 +9060,303 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D2" s="15" t="s">
+        <v>495</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="G4" s="10" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="G5" s="10" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="F4" t="s">
+      <c r="D6" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="C5" t="s">
-        <v>296</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C11" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="C6" t="s">
-        <v>296</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="C12" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="C7" t="s">
-        <v>296</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="C13" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="C8" t="s">
-        <v>296</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="C14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="C9" t="s">
-        <v>303</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="C15" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B10" t="s">
-        <v>295</v>
-      </c>
-      <c r="C10" t="s">
-        <v>303</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="B11" t="s">
-        <v>295</v>
-      </c>
-      <c r="C11" t="s">
-        <v>303</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="B12" t="s">
-        <v>295</v>
-      </c>
-      <c r="C12" t="s">
-        <v>303</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="B13" t="s">
-        <v>295</v>
-      </c>
-      <c r="C13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="B14" t="s">
-        <v>295</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
+      <c r="G15" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A6" r:id="rId4"/>
-    <hyperlink ref="A7" r:id="rId5"/>
-    <hyperlink ref="A8" r:id="rId6"/>
-    <hyperlink ref="A9" r:id="rId7"/>
-    <hyperlink ref="A10" r:id="rId8"/>
-    <hyperlink ref="A11" r:id="rId9"/>
-    <hyperlink ref="A12" r:id="rId10"/>
-    <hyperlink ref="A13" r:id="rId11"/>
-    <hyperlink ref="A14" r:id="rId12"/>
+    <hyperlink ref="A7" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A9" r:id="rId6"/>
+    <hyperlink ref="A10" r:id="rId7"/>
+    <hyperlink ref="A11" r:id="rId8"/>
+    <hyperlink ref="A12" r:id="rId9"/>
+    <hyperlink ref="A13" r:id="rId10"/>
+    <hyperlink ref="A14" r:id="rId11"/>
+    <hyperlink ref="A15" r:id="rId12"/>
     <hyperlink ref="A5" r:id="rId13"/>
+    <hyperlink ref="A8" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -9219,7 +9365,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9245,7 +9391,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
@@ -9259,13 +9405,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" t="s">
         <v>311</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>312</v>
-      </c>
-      <c r="C2" t="s">
-        <v>313</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -9273,13 +9419,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C3" t="s">
         <v>312</v>
-      </c>
-      <c r="C3" t="s">
-        <v>313</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -9287,13 +9433,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C4" t="s">
         <v>312</v>
-      </c>
-      <c r="C4" t="s">
-        <v>313</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -9301,13 +9447,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C5" t="s">
         <v>312</v>
-      </c>
-      <c r="C5" t="s">
-        <v>313</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -9315,13 +9461,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" t="s">
         <v>312</v>
-      </c>
-      <c r="C6" t="s">
-        <v>313</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -9329,13 +9475,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C7" t="s">
         <v>312</v>
-      </c>
-      <c r="C7" t="s">
-        <v>313</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -9343,13 +9489,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B8" t="s">
+        <v>311</v>
+      </c>
+      <c r="C8" t="s">
         <v>319</v>
-      </c>
-      <c r="B8" t="s">
-        <v>312</v>
-      </c>
-      <c r="C8" t="s">
-        <v>320</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -9357,13 +9503,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
@@ -9371,13 +9517,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
@@ -9385,13 +9531,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -9399,13 +9545,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -9413,10 +9559,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C13" t="s">
         <v>203</v>
@@ -9427,10 +9573,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C14" t="s">
         <v>203</v>
@@ -9441,10 +9587,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C15" t="s">
         <v>203</v>
@@ -9455,13 +9601,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="B16" t="s">
+        <v>311</v>
+      </c>
+      <c r="C16" t="s">
         <v>328</v>
-      </c>
-      <c r="B16" t="s">
-        <v>312</v>
-      </c>
-      <c r="C16" t="s">
-        <v>329</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -9469,13 +9615,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
@@ -9483,13 +9629,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F18" t="s">
         <v>17</v>
@@ -9497,13 +9643,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -9511,13 +9657,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C20" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F20" t="s">
         <v>17</v>
@@ -9526,13 +9672,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -9540,13 +9686,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C22" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F22" t="s">
         <v>17</v>
@@ -9554,13 +9700,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
@@ -9568,13 +9714,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B24" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C24" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F24" t="s">
         <v>17</v>
@@ -9582,10 +9728,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C25" t="s">
         <v>76</v>
@@ -9596,10 +9742,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C26" t="s">
         <v>76</v>
@@ -9610,10 +9756,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C27" t="s">
         <v>76</v>
@@ -9624,10 +9770,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C28" t="s">
         <v>76</v>
@@ -9638,10 +9784,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C29" t="s">
         <v>76</v>
@@ -9652,10 +9798,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C30" t="s">
         <v>76</v>
@@ -9666,10 +9812,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C31" t="s">
         <v>76</v>
@@ -9680,10 +9826,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B32" t="s">
         <v>311</v>
-      </c>
-      <c r="B32" t="s">
-        <v>312</v>
       </c>
       <c r="C32" t="s">
         <v>76</v>
@@ -9694,10 +9840,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C33" t="s">
         <v>76</v>
@@ -9708,10 +9854,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C34" t="s">
         <v>65</v>
@@ -9722,10 +9868,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C35" t="s">
         <v>65</v>
@@ -9736,10 +9882,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B36" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C36" t="s">
         <v>65</v>
@@ -9750,10 +9896,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B37" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C37" t="s">
         <v>65</v>
@@ -9764,10 +9910,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C38" t="s">
         <v>65</v>
@@ -9778,10 +9924,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B39" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C39" t="s">
         <v>65</v>
@@ -9792,10 +9938,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B40" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C40" t="s">
         <v>65</v>
@@ -9890,7 +10036,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>4</v>
@@ -9907,43 +10053,43 @@
         <v>175</v>
       </c>
       <c r="B2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C2" t="s">
         <v>354</v>
-      </c>
-      <c r="C2" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="B4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C4" t="s">
         <v>357</v>
-      </c>
-      <c r="B4" t="s">
-        <v>354</v>
-      </c>
-      <c r="C4" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C5" t="s">
         <v>359</v>
-      </c>
-      <c r="B5" t="s">
-        <v>354</v>
-      </c>
-      <c r="C5" t="s">
-        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -9973,427 +10119,427 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -10503,106 +10649,106 @@
   <sheetData>
     <row r="1" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>363</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>382</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="B13" t="s">
         <v>384</v>
-      </c>
-      <c r="B13" t="s">
-        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gitignore lock xls and SUmmation.java
</commit_message>
<xml_diff>
--- a/resources/BinaryTrees.xlsx
+++ b/resources/BinaryTrees.xlsx
@@ -18,6 +18,7 @@
     <sheet name="Tips" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Summation!$A$1:$G$40</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">TraversalAndView!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">ConstructionAndConversion!$A$1:$G$33</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">CheckingAndPrinting!$A$1:$G$67</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="518">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -1144,24 +1145,27 @@
     <t xml:space="preserve">Find sum of all right leaves in a given Binary Tree</t>
   </si>
   <si>
+    <t xml:space="preserve">Find maximum level sum in Binary Tree </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level Depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difference between sums of odd level and even level nodes of a Binary Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of nodes at k-th level in a tree represented as string </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of leaf nodes at minimum level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of heights of all individual nodes in a binary tree </t>
+  </si>
+  <si>
     <t xml:space="preserve">Sum of nodes at maximum depth of a Binary Tree </t>
   </si>
   <si>
-    <t xml:space="preserve">Level Depth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Find maximum level sum in Binary Tree </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sum of leaf nodes at minimum level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sum of nodes at k-th level in a tree represented as string </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sum of heights of all individual nodes in a binary tree </t>
-  </si>
-  <si>
     <t xml:space="preserve">Find largest subtree sum in a tree </t>
   </si>
   <si>
@@ -1228,22 +1232,34 @@
     <t xml:space="preserve">Find root of the tree where children id sum for every node is given </t>
   </si>
   <si>
+    <t xml:space="preserve">findRootOfTheTreeWhereChildrenIdSumForEveryNodeIsGiven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of all node ids – sum of all children id sum</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sum of all the parent nodes having child node x </t>
   </si>
   <si>
+    <t xml:space="preserve">findSumOfAllParentNodesHavingGivenChildNode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal Traversal with check at each node</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Two Binary Trees by doing Node Sum (Recursive and Iterative) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replace each node in binary tree with the sum of its inorder predecessor and successor </t>
+  </si>
+  <si>
     <t xml:space="preserve">Remove all nodes which don’t lie in any path with sum&gt;= k</t>
   </si>
   <si>
+    <t xml:space="preserve">K-Sum</t>
+  </si>
+  <si>
     <t xml:space="preserve">Print all k-sum paths in a binary tree </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Difference between sums of odd level and even level nodes of a Binary Tree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merge Two Binary Trees by doing Node Sum (Recursive and Iterative) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Replace each node in binary tree with the sum of its inorder predecessor and successor </t>
   </si>
   <si>
     <t xml:space="preserve">Github:NaryTrees</t>
@@ -1932,6 +1948,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -7834,7 +7854,7 @@
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.85"/>
@@ -8205,18 +8225,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="80.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.28"/>
@@ -8344,7 +8364,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>363</v>
       </c>
@@ -8408,7 +8428,7 @@
         <v>354</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>203</v>
+        <v>362</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>17</v>
@@ -8450,7 +8470,7 @@
         <v>354</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>371</v>
+        <v>203</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>17</v>
@@ -8458,13 +8478,13 @@
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>354</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>17</v>
@@ -8478,7 +8498,7 @@
         <v>354</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>17</v>
@@ -8492,7 +8512,7 @@
         <v>354</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>17</v>
@@ -8506,12 +8526,11 @@
         <v>354</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
@@ -8521,11 +8540,12 @@
         <v>354</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
@@ -8535,7 +8555,7 @@
         <v>354</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>17</v>
@@ -8549,7 +8569,7 @@
         <v>354</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>17</v>
@@ -8563,7 +8583,7 @@
         <v>354</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>17</v>
@@ -8577,7 +8597,7 @@
         <v>354</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>76</v>
+        <v>372</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>17</v>
@@ -8669,7 +8689,7 @@
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>353</v>
+        <v>387</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>354</v>
@@ -8683,7 +8703,7 @@
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>387</v>
+        <v>353</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>354</v>
@@ -8703,7 +8723,7 @@
         <v>354</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>17</v>
@@ -8719,13 +8739,22 @@
       <c r="C35" s="0" t="s">
         <v>65</v>
       </c>
+      <c r="D35" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>205</v>
+      </c>
       <c r="F35" s="0" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>354</v>
@@ -8733,13 +8762,22 @@
       <c r="C36" s="0" t="s">
         <v>65</v>
       </c>
+      <c r="D36" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>205</v>
+      </c>
       <c r="F36" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>354</v>
@@ -8753,7 +8791,7 @@
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>354</v>
@@ -8765,15 +8803,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>354</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>65</v>
+        <v>398</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>17</v>
@@ -8781,37 +8819,33 @@
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>354</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>65</v>
+        <v>398</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="12"/>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="12"/>
-    </row>
-    <row r="51" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="13"/>
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="13"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G40"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1040" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F40 F42 F52:F1040" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E1040" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E40 E42 E52:E1040" type="list">
       <formula1>"Easy,Medium,Hard"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8823,39 +8857,39 @@
     <hyperlink ref="A5" r:id="rId4" display="Sum of all leaf nodes of binary tree"/>
     <hyperlink ref="A6" r:id="rId5" display="Find sum of all left leaves in a given Binary Tree"/>
     <hyperlink ref="A7" r:id="rId6" display="Find sum of all right leaves in a given Binary Tree"/>
-    <hyperlink ref="A8" r:id="rId7" display="Sum of nodes at maximum depth of a Binary Tree "/>
-    <hyperlink ref="A9" r:id="rId8" display="Find maximum level sum in Binary Tree "/>
-    <hyperlink ref="A10" r:id="rId9" display="Sum of leaf nodes at minimum level"/>
-    <hyperlink ref="A11" r:id="rId10" display="Sum of nodes at k-th level in a tree represented as string "/>
+    <hyperlink ref="A8" r:id="rId7" display="Find maximum level sum in Binary Tree "/>
+    <hyperlink ref="A9" r:id="rId8" display="Difference between sums of odd level and even level nodes of a Binary Tree"/>
+    <hyperlink ref="A10" r:id="rId9" display="Sum of nodes at k-th level in a tree represented as string "/>
+    <hyperlink ref="A11" r:id="rId10" display="Sum of leaf nodes at minimum level"/>
     <hyperlink ref="A12" r:id="rId11" display="Sum of heights of all individual nodes in a binary tree "/>
-    <hyperlink ref="A13" r:id="rId12" display="Find largest subtree sum in a tree "/>
-    <hyperlink ref="A14" r:id="rId13" display="Subtree with given sum in a Binary Tree "/>
-    <hyperlink ref="A15" r:id="rId14" display="Count subtress that sum up to a given value x "/>
-    <hyperlink ref="A16" r:id="rId15" display="Sum of all the numbers that are formed from root to leaf paths"/>
-    <hyperlink ref="A17" r:id="rId16" display="Sum of nodes on the longest path from root to leaf node "/>
-    <hyperlink ref="A18" r:id="rId17" display="Root to leaf path sum equal to a given number"/>
-    <hyperlink ref="A19" r:id="rId18" display="Maximum spiral sum in Binary Tree "/>
-    <hyperlink ref="A20" r:id="rId19" display="Maximum sum of nodes in Binary tree such that no two are adjacent "/>
-    <hyperlink ref="A21" r:id="rId20" display="Maximum sum from a tree with adjacent levels not allowed "/>
-    <hyperlink ref="A22" r:id="rId21" display="Find the maximum sum leaf to root path in a Binary Tree"/>
-    <hyperlink ref="A23" r:id="rId22" display="Find the maximum path sum between two leaves of a binary tree"/>
-    <hyperlink ref="A24" r:id="rId23" display="Find if there is a pair in root to a leaf path with sum equals to root’s data"/>
-    <hyperlink ref="A25" r:id="rId24" display="Sum of nodes in top view of binary tree"/>
-    <hyperlink ref="A26" r:id="rId25" display="Sum of nodes in bottom view of Binary Tree"/>
-    <hyperlink ref="A27" r:id="rId26" display="Sum of nodes in the left view of the given binary tree"/>
-    <hyperlink ref="A28" r:id="rId27" display="Sum of nodes in the right view of the given binary tree"/>
-    <hyperlink ref="A29" r:id="rId28" display="Vertical Sum in a given Binary Tree | Set 1"/>
-    <hyperlink ref="A30" r:id="rId29" display="Vertical Sum in Binary Tree "/>
-    <hyperlink ref="A31" r:id="rId30" display="Diagonal Sum of a Binary Tree"/>
-    <hyperlink ref="A32" r:id="rId31" display="Sum of all nodes in a binary tree"/>
-    <hyperlink ref="A33" r:id="rId32" display="Sum of all the Boundary Nodes of a Binary Tree"/>
-    <hyperlink ref="A34" r:id="rId33" display="Find root of the tree where children id sum for every node is given "/>
-    <hyperlink ref="A35" r:id="rId34" display="Sum of all the parent nodes having child node x "/>
-    <hyperlink ref="A36" r:id="rId35" display="Remove all nodes which don’t lie in any path with sum&gt;= k"/>
-    <hyperlink ref="A37" r:id="rId36" display="Print all k-sum paths in a binary tree "/>
-    <hyperlink ref="A38" r:id="rId37" display="Difference between sums of odd level and even level nodes of a Binary Tree"/>
-    <hyperlink ref="A39" r:id="rId38" display="Merge Two Binary Trees by doing Node Sum (Recursive and Iterative) "/>
-    <hyperlink ref="A40" r:id="rId39" display="Replace each node in binary tree with the sum of its inorder predecessor and successor "/>
+    <hyperlink ref="A13" r:id="rId12" display="Sum of nodes at maximum depth of a Binary Tree "/>
+    <hyperlink ref="A14" r:id="rId13" display="Find largest subtree sum in a tree "/>
+    <hyperlink ref="A15" r:id="rId14" display="Subtree with given sum in a Binary Tree "/>
+    <hyperlink ref="A16" r:id="rId15" display="Count subtress that sum up to a given value x "/>
+    <hyperlink ref="A17" r:id="rId16" display="Sum of all the numbers that are formed from root to leaf paths"/>
+    <hyperlink ref="A18" r:id="rId17" display="Sum of nodes on the longest path from root to leaf node "/>
+    <hyperlink ref="A19" r:id="rId18" display="Root to leaf path sum equal to a given number"/>
+    <hyperlink ref="A20" r:id="rId19" display="Maximum spiral sum in Binary Tree "/>
+    <hyperlink ref="A21" r:id="rId20" display="Maximum sum of nodes in Binary tree such that no two are adjacent "/>
+    <hyperlink ref="A22" r:id="rId21" display="Maximum sum from a tree with adjacent levels not allowed "/>
+    <hyperlink ref="A23" r:id="rId22" display="Find the maximum sum leaf to root path in a Binary Tree"/>
+    <hyperlink ref="A24" r:id="rId23" display="Find the maximum path sum between two leaves of a binary tree"/>
+    <hyperlink ref="A25" r:id="rId24" display="Find if there is a pair in root to a leaf path with sum equals to root’s data"/>
+    <hyperlink ref="A26" r:id="rId25" display="Sum of nodes in top view of binary tree"/>
+    <hyperlink ref="A27" r:id="rId26" display="Sum of nodes in bottom view of Binary Tree"/>
+    <hyperlink ref="A28" r:id="rId27" display="Sum of nodes in the left view of the given binary tree"/>
+    <hyperlink ref="A29" r:id="rId28" display="Sum of nodes in the right view of the given binary tree"/>
+    <hyperlink ref="A30" r:id="rId29" display="Vertical Sum in a given Binary Tree | Set 1"/>
+    <hyperlink ref="A31" r:id="rId30" display="Vertical Sum in Binary Tree "/>
+    <hyperlink ref="A32" r:id="rId31" display="Diagonal Sum of a Binary Tree"/>
+    <hyperlink ref="A33" r:id="rId32" display="Sum of all nodes in a binary tree"/>
+    <hyperlink ref="A34" r:id="rId33" display="Sum of all the Boundary Nodes of a Binary Tree"/>
+    <hyperlink ref="A35" r:id="rId34" display="Find root of the tree where children id sum for every node is given "/>
+    <hyperlink ref="A36" r:id="rId35" display="Sum of all the parent nodes having child node x "/>
+    <hyperlink ref="A37" r:id="rId36" display="Merge Two Binary Trees by doing Node Sum (Recursive and Iterative) "/>
+    <hyperlink ref="A38" r:id="rId37" display="Replace each node in binary tree with the sum of its inorder predecessor and successor "/>
+    <hyperlink ref="A39" r:id="rId38" display="Remove all nodes which don’t lie in any path with sum&gt;= k"/>
+    <hyperlink ref="A40" r:id="rId39" display="Print all k-sum paths in a binary tree "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -8864,6 +8898,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId40"/>
 </worksheet>
 </file>
 
@@ -8878,7 +8913,7 @@
       <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
@@ -8897,7 +8932,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>4</v>
@@ -8914,43 +8949,43 @@
         <v>175</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>401</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="C5" s="0" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -8981,434 +9016,434 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="62.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="11" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="11" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="11" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="11" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="11" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="11" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="11" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="11" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="11" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="11" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="11" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="11" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="11" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="11" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="11" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="11" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="11" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="11" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="11" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="11" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="11" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="11" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="11" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="11" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="11" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="11" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="11" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="11" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="11" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -9520,7 +9555,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.14"/>
@@ -9528,106 +9563,106 @@
   <sheetData>
     <row r="1" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adde dMax path sum in BInaryTrees.xls
</commit_message>
<xml_diff>
--- a/resources/BinaryTrees.xlsx
+++ b/resources/BinaryTrees.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TraversalAndView" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,11 +18,11 @@
     <sheet name="Tips" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Summation!$A$1:$G$41</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">TraversalAndView!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">ConstructionAndConversion!$A$1:$G$33</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">CheckingAndPrinting!$A$1:$G$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Summation!$A$1:$G$40</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Summation!$A$1:$G$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Summation!$A$1:$G$41</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'N-ary Trees'!$A$1:$G$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="535">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -1207,6 +1207,9 @@
   </si>
   <si>
     <t xml:space="preserve">Find the maximum sum leaf to root path in a Binary Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum Path Sum in a Binary Tree</t>
   </si>
   <si>
     <t xml:space="preserve">Find the maximum path sum between two leaves of a binary tree</t>
@@ -1771,7 +1774,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1809,6 +1812,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1864,7 +1874,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1913,7 +1923,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1992,10 +2006,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8268,13 +8278,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8312,7 +8322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>353</v>
       </c>
@@ -8326,7 +8336,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>356</v>
       </c>
@@ -8340,7 +8350,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>357</v>
       </c>
@@ -8354,7 +8364,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>358</v>
       </c>
@@ -8368,7 +8378,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>359</v>
       </c>
@@ -8382,7 +8392,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>360</v>
       </c>
@@ -8498,7 +8508,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
         <v>371</v>
       </c>
@@ -8512,7 +8522,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
         <v>372</v>
       </c>
@@ -8526,7 +8536,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
         <v>373</v>
       </c>
@@ -8540,7 +8550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
         <v>374</v>
       </c>
@@ -8554,7 +8564,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
         <v>376</v>
       </c>
@@ -8568,7 +8578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
         <v>377</v>
       </c>
@@ -8582,7 +8592,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
         <v>378</v>
       </c>
@@ -8596,7 +8606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
         <v>379</v>
       </c>
@@ -8611,7 +8621,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
         <v>380</v>
       </c>
@@ -8625,7 +8635,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
         <v>381</v>
       </c>
@@ -8639,8 +8649,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="12" t="s">
         <v>382</v>
       </c>
       <c r="B24" s="0" t="s">
@@ -8653,7 +8663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
         <v>383</v>
       </c>
@@ -8667,7 +8677,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
         <v>384</v>
       </c>
@@ -8675,13 +8685,13 @@
         <v>354</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>76</v>
+        <v>375</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
         <v>385</v>
       </c>
@@ -8695,7 +8705,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
         <v>386</v>
       </c>
@@ -8709,7 +8719,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
         <v>387</v>
       </c>
@@ -8723,7 +8733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
         <v>388</v>
       </c>
@@ -8737,7 +8747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
         <v>389</v>
       </c>
@@ -8751,7 +8761,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
         <v>390</v>
       </c>
@@ -8765,9 +8775,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>353</v>
+        <v>391</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>354</v>
@@ -8779,9 +8789,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>391</v>
+        <v>353</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>354</v>
@@ -8793,7 +8803,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
         <v>392</v>
       </c>
@@ -8801,24 +8811,15 @@
         <v>354</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7" t="s">
         <v>393</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
-        <v>395</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>354</v>
@@ -8827,7 +8828,7 @@
         <v>65</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>205</v>
@@ -8836,12 +8837,12 @@
         <v>11</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="28.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>354</v>
@@ -8849,8 +8850,8 @@
       <c r="C37" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>399</v>
+      <c r="D37" s="0" t="s">
+        <v>397</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>205</v>
@@ -8859,12 +8860,12 @@
         <v>11</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="28.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>354</v>
@@ -8873,7 +8874,7 @@
         <v>65</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>205</v>
@@ -8882,21 +8883,21 @@
         <v>11</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>404</v>
+        <v>401</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="s">
+        <v>402</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>354</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>406</v>
+        <v>65</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>403</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>205</v>
@@ -8905,21 +8906,21 @@
         <v>11</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
-        <v>408</v>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>405</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>354</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>205</v>
@@ -8928,21 +8929,21 @@
         <v>11</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>354</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>205</v>
@@ -8951,28 +8952,45 @@
         <v>11</v>
       </c>
       <c r="G41" s="0" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="D42" s="0" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="12"/>
-    </row>
+      <c r="E42" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="13"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:G41">
-    <filterColumn colId="2">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Level Depth"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F41 F52:F1040" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F42 F53:F1041" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E41 E52:E1040" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E42 E53:E1041" type="list">
       <formula1>"Easy,Medium,Hard"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9000,24 +9018,25 @@
     <hyperlink ref="A21" r:id="rId20" display="Maximum sum of nodes in Binary tree such that no two are adjacent "/>
     <hyperlink ref="A22" r:id="rId21" display="Maximum sum from a tree with adjacent levels not allowed "/>
     <hyperlink ref="A23" r:id="rId22" display="Find the maximum sum leaf to root path in a Binary Tree"/>
-    <hyperlink ref="A24" r:id="rId23" display="Find the maximum path sum between two leaves of a binary tree"/>
-    <hyperlink ref="A25" r:id="rId24" display="Find if there is a pair in root to a leaf path with sum equals to root’s data"/>
-    <hyperlink ref="A26" r:id="rId25" display="Sum of nodes in top view of binary tree"/>
-    <hyperlink ref="A27" r:id="rId26" display="Sum of nodes in bottom view of Binary Tree"/>
-    <hyperlink ref="A28" r:id="rId27" display="Sum of nodes in the left view of the given binary tree"/>
-    <hyperlink ref="A29" r:id="rId28" display="Sum of nodes in the right view of the given binary tree"/>
-    <hyperlink ref="A30" r:id="rId29" display="Vertical Sum in a given Binary Tree | Set 1"/>
-    <hyperlink ref="A31" r:id="rId30" display="Vertical Sum in Binary Tree "/>
-    <hyperlink ref="A32" r:id="rId31" display="Diagonal Sum of a Binary Tree"/>
-    <hyperlink ref="A33" r:id="rId32" display="Sum of all nodes in a binary tree"/>
-    <hyperlink ref="A34" r:id="rId33" display="Sum of all the Boundary Nodes of a Binary Tree"/>
-    <hyperlink ref="A35" r:id="rId34" display="Find root of the tree where children id sum for every node is given "/>
-    <hyperlink ref="A36" r:id="rId35" display="Sum of all the parent nodes having child node x "/>
-    <hyperlink ref="A37" r:id="rId36" display="Merge Two Binary Trees by doing Node Sum (Recursive and Iterative) "/>
-    <hyperlink ref="A38" r:id="rId37" display="Replace each node in binary tree with the sum of its inorder predecessor and successor "/>
-    <hyperlink ref="A39" r:id="rId38" display="Print all the paths from root, with a specified sum in Binary tree"/>
-    <hyperlink ref="A40" r:id="rId39" display="Print all k-sum paths in a binary tree "/>
-    <hyperlink ref="A41" r:id="rId40" display="Remove all nodes which don’t lie in any path with sum&gt;= k"/>
+    <hyperlink ref="A24" r:id="rId23" display="Maximum Path Sum in a Binary Tree"/>
+    <hyperlink ref="A25" r:id="rId24" display="Find the maximum path sum between two leaves of a binary tree"/>
+    <hyperlink ref="A26" r:id="rId25" display="Find if there is a pair in root to a leaf path with sum equals to root’s data"/>
+    <hyperlink ref="A27" r:id="rId26" display="Sum of nodes in top view of binary tree"/>
+    <hyperlink ref="A28" r:id="rId27" display="Sum of nodes in bottom view of Binary Tree"/>
+    <hyperlink ref="A29" r:id="rId28" display="Sum of nodes in the left view of the given binary tree"/>
+    <hyperlink ref="A30" r:id="rId29" display="Sum of nodes in the right view of the given binary tree"/>
+    <hyperlink ref="A31" r:id="rId30" display="Vertical Sum in a given Binary Tree | Set 1"/>
+    <hyperlink ref="A32" r:id="rId31" display="Vertical Sum in Binary Tree "/>
+    <hyperlink ref="A33" r:id="rId32" display="Diagonal Sum of a Binary Tree"/>
+    <hyperlink ref="A34" r:id="rId33" display="Sum of all nodes in a binary tree"/>
+    <hyperlink ref="A35" r:id="rId34" display="Sum of all the Boundary Nodes of a Binary Tree"/>
+    <hyperlink ref="A36" r:id="rId35" display="Find root of the tree where children id sum for every node is given "/>
+    <hyperlink ref="A37" r:id="rId36" display="Sum of all the parent nodes having child node x "/>
+    <hyperlink ref="A38" r:id="rId37" display="Merge Two Binary Trees by doing Node Sum (Recursive and Iterative) "/>
+    <hyperlink ref="A39" r:id="rId38" display="Replace each node in binary tree with the sum of its inorder predecessor and successor "/>
+    <hyperlink ref="A40" r:id="rId39" display="Print all the paths from root, with a specified sum in Binary tree"/>
+    <hyperlink ref="A41" r:id="rId40" display="Print all k-sum paths in a binary tree "/>
+    <hyperlink ref="A42" r:id="rId41" display="Remove all nodes which don’t lie in any path with sum&gt;= k"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -9026,7 +9045,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId41"/>
 </worksheet>
 </file>
 
@@ -9060,7 +9078,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>4</v>
@@ -9077,43 +9095,43 @@
         <v>175</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -9151,427 +9169,427 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="11" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="11" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="11" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="11" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="11" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="11" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="11" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="11" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="11" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="11" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="11" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="11" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="11" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="11" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="11" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="11" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="11" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="11" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="11" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="11" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="11" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="11" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="11" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="11" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="11" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="11" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="11" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="11" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="11" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -9679,8 +9697,8 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9691,114 +9709,114 @@
   <sheetData>
     <row r="1" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
-        <v>530</v>
+      <c r="A13" s="14" t="s">
+        <v>531</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>